<commit_message>
Start creating glass type DB
</commit_message>
<xml_diff>
--- a/glassdata/GlassTypes-202505.xlsx
+++ b/glassdata/GlassTypes-202505.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dylan\git\Beam42\glassdata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8E8CECF9-181E-4FD3-ACC9-CF835ADC42EB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C8F07FDD-866B-46F3-BA77-27220E8AA963}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="51840" windowHeight="21120" xr2:uid="{A1152BF3-FB9E-42F0-86FF-96184CF2F371}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1282" uniqueCount="691">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1550" uniqueCount="826">
   <si>
     <t>Make</t>
   </si>
@@ -2109,6 +2109,411 @@
   </si>
   <si>
     <t>Rel Price</t>
+  </si>
+  <si>
+    <t>Ohara</t>
+  </si>
+  <si>
+    <t>S-FPL51</t>
+  </si>
+  <si>
+    <t>S-FPL53</t>
+  </si>
+  <si>
+    <t>S-FPL55</t>
+  </si>
+  <si>
+    <t>S-BSM10</t>
+  </si>
+  <si>
+    <t>S-BSM14</t>
+  </si>
+  <si>
+    <t>S-BSM15</t>
+  </si>
+  <si>
+    <t>S-BSM16</t>
+  </si>
+  <si>
+    <t>S-BSM18</t>
+  </si>
+  <si>
+    <t>S-BSM25</t>
+  </si>
+  <si>
+    <t>S-BSM28</t>
+  </si>
+  <si>
+    <t>S-BSM71</t>
+  </si>
+  <si>
+    <t>S-BSM81</t>
+  </si>
+  <si>
+    <t>S-NSL36</t>
+  </si>
+  <si>
+    <t>S-BAL12</t>
+  </si>
+  <si>
+    <t>S-BAL14</t>
+  </si>
+  <si>
+    <t>S-BAL35</t>
+  </si>
+  <si>
+    <t>S-BAL42</t>
+  </si>
+  <si>
+    <t>S-BAM12</t>
+  </si>
+  <si>
+    <t>S-BAH11</t>
+  </si>
+  <si>
+    <t>S-BAH27</t>
+  </si>
+  <si>
+    <t>S-BAH28</t>
+  </si>
+  <si>
+    <t>S-PHM52</t>
+  </si>
+  <si>
+    <t>S-PHM52Q</t>
+  </si>
+  <si>
+    <t>S-PHM53</t>
+  </si>
+  <si>
+    <t>S-TIL25</t>
+  </si>
+  <si>
+    <t>S-TIL26</t>
+  </si>
+  <si>
+    <t>S-TIL27</t>
+  </si>
+  <si>
+    <t>S-TIM25</t>
+  </si>
+  <si>
+    <t>S-TIM27</t>
+  </si>
+  <si>
+    <t>S-TIM28</t>
+  </si>
+  <si>
+    <t>S-TIM35</t>
+  </si>
+  <si>
+    <t>S-TIH10</t>
+  </si>
+  <si>
+    <t>S-TIH11</t>
+  </si>
+  <si>
+    <t>S-TIH13</t>
+  </si>
+  <si>
+    <t>S-TIH14</t>
+  </si>
+  <si>
+    <t>S-TIH18</t>
+  </si>
+  <si>
+    <t>S-TIH53</t>
+  </si>
+  <si>
+    <t>S-TIH53W</t>
+  </si>
+  <si>
+    <t>S-TIH53WN</t>
+  </si>
+  <si>
+    <t>S-TIH57</t>
+  </si>
+  <si>
+    <t>S-LAL10</t>
+  </si>
+  <si>
+    <t>S-LAL12</t>
+  </si>
+  <si>
+    <t>S-LAL12Q</t>
+  </si>
+  <si>
+    <t>S-LAL14</t>
+  </si>
+  <si>
+    <t>S-LAL18</t>
+  </si>
+  <si>
+    <t>S-LAL18N</t>
+  </si>
+  <si>
+    <t>S-LAL19</t>
+  </si>
+  <si>
+    <t>S-LAL20</t>
+  </si>
+  <si>
+    <t>S-LAL21</t>
+  </si>
+  <si>
+    <t>S-LAL54Q</t>
+  </si>
+  <si>
+    <t>S-LAL58</t>
+  </si>
+  <si>
+    <t>S-LAL59</t>
+  </si>
+  <si>
+    <t>S-LAL61</t>
+  </si>
+  <si>
+    <t>S-LAL61Q</t>
+  </si>
+  <si>
+    <t>S-LAM55</t>
+  </si>
+  <si>
+    <t>S-LAM60</t>
+  </si>
+  <si>
+    <t>S-LAM66</t>
+  </si>
+  <si>
+    <t>S-LAM73</t>
+  </si>
+  <si>
+    <t>S-LAH51</t>
+  </si>
+  <si>
+    <t>S-LAH52</t>
+  </si>
+  <si>
+    <t>S-LAH52Q</t>
+  </si>
+  <si>
+    <t>S-LAH53</t>
+  </si>
+  <si>
+    <t>S-LAH53V</t>
+  </si>
+  <si>
+    <t>S-LAH55V</t>
+  </si>
+  <si>
+    <t>S-LAH55VS</t>
+  </si>
+  <si>
+    <t>S-LAH58</t>
+  </si>
+  <si>
+    <t>S-LAH59</t>
+  </si>
+  <si>
+    <t>S-LAH60</t>
+  </si>
+  <si>
+    <t>S-LAH60MQ</t>
+  </si>
+  <si>
+    <t>S-LAH60V</t>
+  </si>
+  <si>
+    <t>S-LAH63Q</t>
+  </si>
+  <si>
+    <t>S-LAH64</t>
+  </si>
+  <si>
+    <t>S-LAH65V</t>
+  </si>
+  <si>
+    <t>S-LAH65VS</t>
+  </si>
+  <si>
+    <t>S-LAH66</t>
+  </si>
+  <si>
+    <t>S-LAH66N</t>
+  </si>
+  <si>
+    <t>S-LAH71</t>
+  </si>
+  <si>
+    <t>S-LAH79</t>
+  </si>
+  <si>
+    <t>S-LAH88</t>
+  </si>
+  <si>
+    <t>S-LAH89</t>
+  </si>
+  <si>
+    <t>S-LAH92</t>
+  </si>
+  <si>
+    <t>S-LAH93</t>
+  </si>
+  <si>
+    <t>S-LAH95</t>
+  </si>
+  <si>
+    <t>S-LAH96</t>
+  </si>
+  <si>
+    <t>S-LAH97</t>
+  </si>
+  <si>
+    <t>S-LAH98</t>
+  </si>
+  <si>
+    <t>S-LAH99</t>
+  </si>
+  <si>
+    <t>S-LAH99W</t>
+  </si>
+  <si>
+    <t>S-FTM16</t>
+  </si>
+  <si>
+    <t>S-NBM51</t>
+  </si>
+  <si>
+    <t>S-NBM52</t>
+  </si>
+  <si>
+    <t>S-NBH51</t>
+  </si>
+  <si>
+    <t>S-NBH52V</t>
+  </si>
+  <si>
+    <t>S-NBH53V</t>
+  </si>
+  <si>
+    <t>S-NBH55</t>
+  </si>
+  <si>
+    <t>S-NBH56</t>
+  </si>
+  <si>
+    <t>S-NBH57</t>
+  </si>
+  <si>
+    <t>S-NBH58</t>
+  </si>
+  <si>
+    <t>S-NBH59</t>
+  </si>
+  <si>
+    <t>S-FPM2</t>
+  </si>
+  <si>
+    <t>S-FPM3</t>
+  </si>
+  <si>
+    <t>S-FPM4</t>
+  </si>
+  <si>
+    <t>S-FPM5</t>
+  </si>
+  <si>
+    <t>S-FSL5</t>
+  </si>
+  <si>
+    <t>S-BSL7</t>
+  </si>
+  <si>
+    <t>S-BSM2</t>
+  </si>
+  <si>
+    <t>S-NSL3</t>
+  </si>
+  <si>
+    <t>S-BAL3</t>
+  </si>
+  <si>
+    <t>S-TIL1</t>
+  </si>
+  <si>
+    <t>S-TIL2</t>
+  </si>
+  <si>
+    <t>S-TIL6</t>
+  </si>
+  <si>
+    <t>S-TIM2</t>
+  </si>
+  <si>
+    <t>S-TIM5</t>
+  </si>
+  <si>
+    <t>S-TIM8</t>
+  </si>
+  <si>
+    <t>S-TIH1</t>
+  </si>
+  <si>
+    <t>S-TIH3</t>
+  </si>
+  <si>
+    <t>S-TIH4</t>
+  </si>
+  <si>
+    <t>S-TIH6</t>
+  </si>
+  <si>
+    <t>S-LAL7Q</t>
+  </si>
+  <si>
+    <t>S-LAL8</t>
+  </si>
+  <si>
+    <t>S-LAL9</t>
+  </si>
+  <si>
+    <t>S-NPH1</t>
+  </si>
+  <si>
+    <t>S-NPH1W</t>
+  </si>
+  <si>
+    <t>S-NPH2</t>
+  </si>
+  <si>
+    <t>S-NPH3</t>
+  </si>
+  <si>
+    <t>S-NPH4</t>
+  </si>
+  <si>
+    <t>S-NPH5</t>
+  </si>
+  <si>
+    <t>S-NPH7</t>
+  </si>
+  <si>
+    <t>S-NBH8</t>
+  </si>
+  <si>
+    <t>S-NBH5</t>
+  </si>
+  <si>
+    <t>S-LAM2</t>
+  </si>
+  <si>
+    <t>S-LAM3</t>
+  </si>
+  <si>
+    <t>S-LAM7</t>
+  </si>
+  <si>
+    <t>S-BAM4</t>
   </si>
 </sst>
 </file>
@@ -2116,7 +2521,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="168" formatCode="_-* #,##0.00\ _€_-;\-* #,##0.00\ _€_-;_-* &quot;-&quot;??\ _€_-;_-@_-"/>
+    <numFmt numFmtId="164" formatCode="_-* #,##0.00\ _€_-;\-* #,##0.00\ _€_-;_-* &quot;-&quot;??\ _€_-;_-@_-"/>
   </numFmts>
   <fonts count="3">
     <font>
@@ -2156,9 +2561,9 @@
   <cellStyleXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
-    <xf numFmtId="168" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
-    <xf numFmtId="168" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
@@ -2500,10 +2905,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9D3D16D4-7B62-4F96-B115-2A44819D0941}">
-  <dimension ref="A1:J520"/>
+  <dimension ref="A1:J654"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A466" workbookViewId="0">
-      <selection activeCell="A521" sqref="A521"/>
+    <sheetView tabSelected="1" topLeftCell="A244" workbookViewId="0">
+      <selection activeCell="U524" sqref="U524"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
@@ -18263,7 +18668,7 @@
         <v>2.7</v>
       </c>
       <c r="J515" t="str">
-        <f t="shared" ref="J515:J520" si="8">CONCATENATE("glasses.put(""",B515,""", new GlassMap(""",A515,""",""",B515,""",",E515,",",D515,",",F515,")); // ",G515, " ",C515," ",H515)</f>
+        <f t="shared" ref="J515:J578" si="8">CONCATENATE("glasses.put(""",B515,""", new GlassMap(""",A515,""",""",B515,""",",E515,",",D515,",",F515,")); // ",G515, " ",C515," ",H515)</f>
         <v>glasses.put(" SF56A ", new GlassMap("Schott"," SF56A ",1.7847,1.77605,1.80615)); // 26.08 785261.492 0.0098</v>
       </c>
     </row>
@@ -18427,6 +18832,4026 @@
       <c r="J520" t="str">
         <f t="shared" si="8"/>
         <v>glasses.put(" SF6HT ", new GlassMap("Schott"," SF6HT ",1.80518,1.79609,1.82775)); // 25.43 805254.518 0.0092</v>
+      </c>
+    </row>
+    <row r="521" spans="1:10">
+      <c r="A521" t="s">
+        <v>691</v>
+      </c>
+      <c r="B521" t="s">
+        <v>692</v>
+      </c>
+      <c r="C521">
+        <v>497816</v>
+      </c>
+      <c r="D521">
+        <v>1.495136</v>
+      </c>
+      <c r="E521">
+        <v>1.496999</v>
+      </c>
+      <c r="F521">
+        <v>1.501231</v>
+      </c>
+      <c r="G521">
+        <v>81.599999999999994</v>
+      </c>
+      <c r="H521">
+        <v>2.8000000000000001E-2</v>
+      </c>
+      <c r="J521" t="str">
+        <f t="shared" si="8"/>
+        <v>glasses.put("S-FPL51", new GlassMap("Ohara","S-FPL51",1.496999,1.495136,1.501231)); // 81.6 497816 0.028</v>
+      </c>
+    </row>
+    <row r="522" spans="1:10">
+      <c r="A522" t="s">
+        <v>691</v>
+      </c>
+      <c r="B522" t="s">
+        <v>693</v>
+      </c>
+      <c r="C522">
+        <v>439950</v>
+      </c>
+      <c r="D522">
+        <v>1.437333</v>
+      </c>
+      <c r="E522">
+        <v>1.43875</v>
+      </c>
+      <c r="F522">
+        <v>1.4419550000000001</v>
+      </c>
+      <c r="G522">
+        <v>95</v>
+      </c>
+      <c r="H522">
+        <v>4.6100000000000002E-2</v>
+      </c>
+      <c r="J522" t="str">
+        <f t="shared" si="8"/>
+        <v>glasses.put("S-FPL53", new GlassMap("Ohara","S-FPL53",1.43875,1.437333,1.441955)); // 95 439950 0.0461</v>
+      </c>
+    </row>
+    <row r="523" spans="1:10">
+      <c r="A523" t="s">
+        <v>691</v>
+      </c>
+      <c r="B523" t="s">
+        <v>694</v>
+      </c>
+      <c r="C523">
+        <v>439948</v>
+      </c>
+      <c r="D523">
+        <v>1.4373279999999999</v>
+      </c>
+      <c r="E523">
+        <v>1.43875</v>
+      </c>
+      <c r="F523">
+        <v>1.4419630000000001</v>
+      </c>
+      <c r="G523">
+        <v>94.8</v>
+      </c>
+      <c r="H523">
+        <v>4.5699999999999998E-2</v>
+      </c>
+      <c r="J523" t="str">
+        <f t="shared" si="8"/>
+        <v>glasses.put("S-FPL55", new GlassMap("Ohara","S-FPL55",1.43875,1.437328,1.441963)); // 94.8 439948 0.0457</v>
+      </c>
+    </row>
+    <row r="524" spans="1:10">
+      <c r="A524" t="s">
+        <v>691</v>
+      </c>
+      <c r="B524" t="s">
+        <v>791</v>
+      </c>
+      <c r="C524">
+        <v>595677</v>
+      </c>
+      <c r="D524">
+        <v>1.5925549999999999</v>
+      </c>
+      <c r="E524">
+        <v>1.5952200000000001</v>
+      </c>
+      <c r="F524">
+        <v>1.601342</v>
+      </c>
+      <c r="G524">
+        <v>67.7</v>
+      </c>
+      <c r="H524">
+        <v>1.23E-2</v>
+      </c>
+      <c r="J524" t="str">
+        <f t="shared" si="8"/>
+        <v>glasses.put("S-FPM2", new GlassMap("Ohara","S-FPM2",1.59522,1.592555,1.601342)); // 67.7 595677 0.0123</v>
+      </c>
+    </row>
+    <row r="525" spans="1:10">
+      <c r="A525" t="s">
+        <v>691</v>
+      </c>
+      <c r="B525" t="s">
+        <v>792</v>
+      </c>
+      <c r="C525">
+        <v>538747</v>
+      </c>
+      <c r="D525">
+        <v>1.5355540000000001</v>
+      </c>
+      <c r="E525">
+        <v>1.53775</v>
+      </c>
+      <c r="F525">
+        <v>1.542753</v>
+      </c>
+      <c r="G525">
+        <v>74.7</v>
+      </c>
+      <c r="H525">
+        <v>1.8599999999999998E-2</v>
+      </c>
+      <c r="J525" t="str">
+        <f t="shared" si="8"/>
+        <v>glasses.put("S-FPM3", new GlassMap("Ohara","S-FPM3",1.53775,1.535554,1.542753)); // 74.7 538747 0.0186</v>
+      </c>
+    </row>
+    <row r="526" spans="1:10">
+      <c r="A526" t="s">
+        <v>691</v>
+      </c>
+      <c r="B526" t="s">
+        <v>793</v>
+      </c>
+      <c r="C526">
+        <v>528765</v>
+      </c>
+      <c r="D526">
+        <v>1.526303</v>
+      </c>
+      <c r="E526">
+        <v>1.52841</v>
+      </c>
+      <c r="F526">
+        <v>1.5332140000000001</v>
+      </c>
+      <c r="G526">
+        <v>76.5</v>
+      </c>
+      <c r="H526">
+        <v>2.18E-2</v>
+      </c>
+      <c r="J526" t="str">
+        <f t="shared" si="8"/>
+        <v>glasses.put("S-FPM4", new GlassMap("Ohara","S-FPM4",1.52841,1.526303,1.533214)); // 76.5 528765 0.0218</v>
+      </c>
+    </row>
+    <row r="527" spans="1:10">
+      <c r="A527" t="s">
+        <v>691</v>
+      </c>
+      <c r="B527" t="s">
+        <v>794</v>
+      </c>
+      <c r="C527">
+        <v>552708</v>
+      </c>
+      <c r="D527">
+        <v>1.549625</v>
+      </c>
+      <c r="E527">
+        <v>1.552</v>
+      </c>
+      <c r="F527">
+        <v>1.5574330000000001</v>
+      </c>
+      <c r="G527">
+        <v>70.8</v>
+      </c>
+      <c r="H527">
+        <v>1.4999999999999999E-2</v>
+      </c>
+      <c r="J527" t="str">
+        <f t="shared" si="8"/>
+        <v>glasses.put("S-FPM5", new GlassMap("Ohara","S-FPM5",1.552,1.549625,1.557433)); // 70.8 552708 0.015</v>
+      </c>
+    </row>
+    <row r="528" spans="1:10">
+      <c r="A528" t="s">
+        <v>691</v>
+      </c>
+      <c r="B528" t="s">
+        <v>795</v>
+      </c>
+      <c r="C528">
+        <v>487702</v>
+      </c>
+      <c r="D528">
+        <v>1.485344</v>
+      </c>
+      <c r="E528">
+        <v>1.48749</v>
+      </c>
+      <c r="F528">
+        <v>1.4922850000000001</v>
+      </c>
+      <c r="G528">
+        <v>70.2</v>
+      </c>
+      <c r="H528">
+        <v>2.2000000000000001E-3</v>
+      </c>
+      <c r="J528" t="str">
+        <f t="shared" si="8"/>
+        <v>glasses.put("S-FSL5", new GlassMap("Ohara","S-FSL5",1.48749,1.485344,1.492285)); // 70.2 487702 0.0022</v>
+      </c>
+    </row>
+    <row r="529" spans="1:10">
+      <c r="A529" t="s">
+        <v>691</v>
+      </c>
+      <c r="B529" t="s">
+        <v>796</v>
+      </c>
+      <c r="C529">
+        <v>516641</v>
+      </c>
+      <c r="D529">
+        <v>1.513855</v>
+      </c>
+      <c r="E529">
+        <v>1.51633</v>
+      </c>
+      <c r="F529">
+        <v>1.5219050000000001</v>
+      </c>
+      <c r="G529">
+        <v>64.099999999999994</v>
+      </c>
+      <c r="H529">
+        <v>-2.3999999999999998E-3</v>
+      </c>
+      <c r="J529" t="str">
+        <f t="shared" si="8"/>
+        <v>glasses.put("S-BSL7", new GlassMap("Ohara","S-BSL7",1.51633,1.513855,1.521905)); // 64.1 516641 -0.0024</v>
+      </c>
+    </row>
+    <row r="530" spans="1:10">
+      <c r="A530" t="s">
+        <v>691</v>
+      </c>
+      <c r="B530" t="s">
+        <v>797</v>
+      </c>
+      <c r="C530">
+        <v>607568</v>
+      </c>
+      <c r="D530">
+        <v>1.604144</v>
+      </c>
+      <c r="E530">
+        <v>1.6073789999999999</v>
+      </c>
+      <c r="F530">
+        <v>1.614835</v>
+      </c>
+      <c r="G530">
+        <v>56.8</v>
+      </c>
+      <c r="H530">
+        <v>-1.2999999999999999E-3</v>
+      </c>
+      <c r="J530" t="str">
+        <f t="shared" si="8"/>
+        <v>glasses.put("S-BSM2", new GlassMap("Ohara","S-BSM2",1.607379,1.604144,1.614835)); // 56.8 607568 -0.0013</v>
+      </c>
+    </row>
+    <row r="531" spans="1:10">
+      <c r="A531" t="s">
+        <v>691</v>
+      </c>
+      <c r="B531" t="s">
+        <v>695</v>
+      </c>
+      <c r="C531">
+        <v>623570</v>
+      </c>
+      <c r="D531">
+        <v>1.619489</v>
+      </c>
+      <c r="E531">
+        <v>1.6227990000000001</v>
+      </c>
+      <c r="F531">
+        <v>1.6304050000000001</v>
+      </c>
+      <c r="G531">
+        <v>57</v>
+      </c>
+      <c r="H531">
+        <v>-2.8E-3</v>
+      </c>
+      <c r="J531" t="str">
+        <f t="shared" si="8"/>
+        <v>glasses.put("S-BSM10", new GlassMap("Ohara","S-BSM10",1.622799,1.619489,1.630405)); // 57 623570 -0.0028</v>
+      </c>
+    </row>
+    <row r="532" spans="1:10">
+      <c r="A532" t="s">
+        <v>691</v>
+      </c>
+      <c r="B532" t="s">
+        <v>696</v>
+      </c>
+      <c r="C532">
+        <v>603607</v>
+      </c>
+      <c r="D532">
+        <v>1.600079</v>
+      </c>
+      <c r="E532">
+        <v>1.6031120000000001</v>
+      </c>
+      <c r="F532">
+        <v>1.6100239999999999</v>
+      </c>
+      <c r="G532">
+        <v>60.7</v>
+      </c>
+      <c r="H532">
+        <v>-1.9E-3</v>
+      </c>
+      <c r="J532" t="str">
+        <f t="shared" si="8"/>
+        <v>glasses.put("S-BSM14", new GlassMap("Ohara","S-BSM14",1.603112,1.600079,1.610024)); // 60.7 603607 -0.0019</v>
+      </c>
+    </row>
+    <row r="533" spans="1:10">
+      <c r="A533" t="s">
+        <v>691</v>
+      </c>
+      <c r="B533" t="s">
+        <v>697</v>
+      </c>
+      <c r="C533">
+        <v>623582</v>
+      </c>
+      <c r="D533">
+        <v>1.619739</v>
+      </c>
+      <c r="E533">
+        <v>1.622992</v>
+      </c>
+      <c r="F533">
+        <v>1.63045</v>
+      </c>
+      <c r="G533">
+        <v>58.2</v>
+      </c>
+      <c r="H533">
+        <v>-1.6000000000000001E-3</v>
+      </c>
+      <c r="J533" t="str">
+        <f t="shared" si="8"/>
+        <v>glasses.put("S-BSM15", new GlassMap("Ohara","S-BSM15",1.622992,1.619739,1.63045)); // 58.2 623582 -0.0016</v>
+      </c>
+    </row>
+    <row r="534" spans="1:10">
+      <c r="A534" t="s">
+        <v>691</v>
+      </c>
+      <c r="B534" t="s">
+        <v>698</v>
+      </c>
+      <c r="C534">
+        <v>620603</v>
+      </c>
+      <c r="D534">
+        <v>1.6172759999999999</v>
+      </c>
+      <c r="E534">
+        <v>1.620411</v>
+      </c>
+      <c r="F534">
+        <v>1.6275660000000001</v>
+      </c>
+      <c r="G534">
+        <v>60.3</v>
+      </c>
+      <c r="H534">
+        <v>-1.1999999999999999E-3</v>
+      </c>
+      <c r="J534" t="str">
+        <f t="shared" si="8"/>
+        <v>glasses.put("S-BSM16", new GlassMap("Ohara","S-BSM16",1.620411,1.617276,1.627566)); // 60.3 620603 -0.0012</v>
+      </c>
+    </row>
+    <row r="535" spans="1:10">
+      <c r="A535" t="s">
+        <v>691</v>
+      </c>
+      <c r="B535" t="s">
+        <v>699</v>
+      </c>
+      <c r="C535">
+        <v>639554</v>
+      </c>
+      <c r="D535">
+        <v>1.635051</v>
+      </c>
+      <c r="E535">
+        <v>1.638539</v>
+      </c>
+      <c r="F535">
+        <v>1.646582</v>
+      </c>
+      <c r="G535">
+        <v>55.4</v>
+      </c>
+      <c r="H535">
+        <v>-3.5000000000000001E-3</v>
+      </c>
+      <c r="J535" t="str">
+        <f t="shared" si="8"/>
+        <v>glasses.put("S-BSM18", new GlassMap("Ohara","S-BSM18",1.638539,1.635051,1.646582)); // 55.4 639554 -0.0035</v>
+      </c>
+    </row>
+    <row r="536" spans="1:10">
+      <c r="A536" t="s">
+        <v>691</v>
+      </c>
+      <c r="B536" t="s">
+        <v>700</v>
+      </c>
+      <c r="C536">
+        <v>658509</v>
+      </c>
+      <c r="D536">
+        <v>1.6545529999999999</v>
+      </c>
+      <c r="E536">
+        <v>1.6584410000000001</v>
+      </c>
+      <c r="F536">
+        <v>1.6674949999999999</v>
+      </c>
+      <c r="G536">
+        <v>50.9</v>
+      </c>
+      <c r="H536">
+        <v>-3.0999999999999999E-3</v>
+      </c>
+      <c r="J536" t="str">
+        <f t="shared" si="8"/>
+        <v>glasses.put("S-BSM25", new GlassMap("Ohara","S-BSM25",1.658441,1.654553,1.667495)); // 50.9 658509 -0.0031</v>
+      </c>
+    </row>
+    <row r="537" spans="1:10">
+      <c r="A537" t="s">
+        <v>691</v>
+      </c>
+      <c r="B537" t="s">
+        <v>701</v>
+      </c>
+      <c r="C537">
+        <v>618498</v>
+      </c>
+      <c r="D537">
+        <v>1.6140049999999999</v>
+      </c>
+      <c r="E537">
+        <v>1.6177220000000001</v>
+      </c>
+      <c r="F537">
+        <v>1.626406</v>
+      </c>
+      <c r="G537">
+        <v>49.8</v>
+      </c>
+      <c r="H537">
+        <v>-5.9999999999999995E-4</v>
+      </c>
+      <c r="J537" t="str">
+        <f t="shared" si="8"/>
+        <v>glasses.put("S-BSM28", new GlassMap("Ohara","S-BSM28",1.617722,1.614005,1.626406)); // 49.8 618498 -0.0006</v>
+      </c>
+    </row>
+    <row r="538" spans="1:10">
+      <c r="A538" t="s">
+        <v>691</v>
+      </c>
+      <c r="B538" t="s">
+        <v>702</v>
+      </c>
+      <c r="C538">
+        <v>649530</v>
+      </c>
+      <c r="D538">
+        <v>1.6448149999999999</v>
+      </c>
+      <c r="E538">
+        <v>1.648498</v>
+      </c>
+      <c r="F538">
+        <v>1.657046</v>
+      </c>
+      <c r="G538">
+        <v>53</v>
+      </c>
+      <c r="H538">
+        <v>-1E-3</v>
+      </c>
+      <c r="J538" t="str">
+        <f t="shared" si="8"/>
+        <v>glasses.put("S-BSM71", new GlassMap("Ohara","S-BSM71",1.648498,1.644815,1.657046)); // 53 649530 -0.001</v>
+      </c>
+    </row>
+    <row r="539" spans="1:10">
+      <c r="A539" t="s">
+        <v>691</v>
+      </c>
+      <c r="B539" t="s">
+        <v>703</v>
+      </c>
+      <c r="C539">
+        <v>640601</v>
+      </c>
+      <c r="D539">
+        <v>1.636728</v>
+      </c>
+      <c r="E539">
+        <v>1.639999</v>
+      </c>
+      <c r="F539">
+        <v>1.647381</v>
+      </c>
+      <c r="G539">
+        <v>60.1</v>
+      </c>
+      <c r="H539">
+        <v>-7.3000000000000001E-3</v>
+      </c>
+      <c r="J539" t="str">
+        <f t="shared" si="8"/>
+        <v>glasses.put("S-BSM81", new GlassMap("Ohara","S-BSM81",1.639999,1.636728,1.647381)); // 60.1 640601 -0.0073</v>
+      </c>
+    </row>
+    <row r="540" spans="1:10">
+      <c r="A540" t="s">
+        <v>691</v>
+      </c>
+      <c r="B540" t="s">
+        <v>798</v>
+      </c>
+      <c r="C540">
+        <v>518590</v>
+      </c>
+      <c r="D540">
+        <v>1.5155559999999999</v>
+      </c>
+      <c r="E540">
+        <v>1.5182290000000001</v>
+      </c>
+      <c r="F540">
+        <v>1.524354</v>
+      </c>
+      <c r="G540">
+        <v>59</v>
+      </c>
+      <c r="H540">
+        <v>-5.0000000000000001E-4</v>
+      </c>
+      <c r="J540" t="str">
+        <f t="shared" si="8"/>
+        <v>glasses.put("S-NSL3", new GlassMap("Ohara","S-NSL3",1.518229,1.515556,1.524354)); // 59 518590 -0.0005</v>
+      </c>
+    </row>
+    <row r="541" spans="1:10">
+      <c r="A541" t="s">
+        <v>691</v>
+      </c>
+      <c r="B541" t="s">
+        <v>704</v>
+      </c>
+      <c r="C541">
+        <v>517524</v>
+      </c>
+      <c r="D541">
+        <v>1.5144439999999999</v>
+      </c>
+      <c r="E541">
+        <v>1.517417</v>
+      </c>
+      <c r="F541">
+        <v>1.524313</v>
+      </c>
+      <c r="G541">
+        <v>52.4</v>
+      </c>
+      <c r="H541">
+        <v>-2.0000000000000001E-4</v>
+      </c>
+      <c r="J541" t="str">
+        <f t="shared" si="8"/>
+        <v>glasses.put("S-NSL36", new GlassMap("Ohara","S-NSL36",1.517417,1.514444,1.524313)); // 52.4 517524 -0.0002</v>
+      </c>
+    </row>
+    <row r="542" spans="1:10">
+      <c r="A542" t="s">
+        <v>691</v>
+      </c>
+      <c r="B542" t="s">
+        <v>799</v>
+      </c>
+      <c r="C542">
+        <v>571530</v>
+      </c>
+      <c r="D542">
+        <v>1.5681050000000001</v>
+      </c>
+      <c r="E542">
+        <v>1.5713509999999999</v>
+      </c>
+      <c r="F542">
+        <v>1.5788949999999999</v>
+      </c>
+      <c r="G542">
+        <v>53</v>
+      </c>
+      <c r="H542">
+        <v>-5.0000000000000001E-4</v>
+      </c>
+      <c r="J542" t="str">
+        <f t="shared" si="8"/>
+        <v>glasses.put("S-BAL3", new GlassMap("Ohara","S-BAL3",1.571351,1.568105,1.578895)); // 53 571530 -0.0005</v>
+      </c>
+    </row>
+    <row r="543" spans="1:10">
+      <c r="A543" t="s">
+        <v>691</v>
+      </c>
+      <c r="B543" t="s">
+        <v>705</v>
+      </c>
+      <c r="C543">
+        <v>540595</v>
+      </c>
+      <c r="D543">
+        <v>1.5371939999999999</v>
+      </c>
+      <c r="E543">
+        <v>1.5399560000000001</v>
+      </c>
+      <c r="F543">
+        <v>1.5462750000000001</v>
+      </c>
+      <c r="G543">
+        <v>59.5</v>
+      </c>
+      <c r="H543">
+        <v>-1.1999999999999999E-3</v>
+      </c>
+      <c r="J543" t="str">
+        <f t="shared" si="8"/>
+        <v>glasses.put("S-BAL12", new GlassMap("Ohara","S-BAL12",1.539956,1.537194,1.546275)); // 59.5 540595 -0.0012</v>
+      </c>
+    </row>
+    <row r="544" spans="1:10">
+      <c r="A544" t="s">
+        <v>691</v>
+      </c>
+      <c r="B544" t="s">
+        <v>706</v>
+      </c>
+      <c r="C544">
+        <v>569563</v>
+      </c>
+      <c r="D544">
+        <v>1.5657749999999999</v>
+      </c>
+      <c r="E544">
+        <v>1.568832</v>
+      </c>
+      <c r="F544">
+        <v>1.5758669999999999</v>
+      </c>
+      <c r="G544">
+        <v>56.3</v>
+      </c>
+      <c r="H544">
+        <v>-1.4E-3</v>
+      </c>
+      <c r="J544" t="str">
+        <f t="shared" si="8"/>
+        <v>glasses.put("S-BAL14", new GlassMap("Ohara","S-BAL14",1.568832,1.565775,1.575867)); // 56.3 569563 -0.0014</v>
+      </c>
+    </row>
+    <row r="545" spans="1:10">
+      <c r="A545" t="s">
+        <v>691</v>
+      </c>
+      <c r="B545" t="s">
+        <v>707</v>
+      </c>
+      <c r="C545">
+        <v>589612</v>
+      </c>
+      <c r="D545">
+        <v>1.5861879999999999</v>
+      </c>
+      <c r="E545">
+        <v>1.5891299999999999</v>
+      </c>
+      <c r="F545">
+        <v>1.5958239999999999</v>
+      </c>
+      <c r="G545">
+        <v>61.2</v>
+      </c>
+      <c r="H545">
+        <v>-1.8E-3</v>
+      </c>
+      <c r="J545" t="str">
+        <f t="shared" si="8"/>
+        <v>glasses.put("S-BAL35", new GlassMap("Ohara","S-BAL35",1.58913,1.586188,1.595824)); // 61.2 589612 -0.0018</v>
+      </c>
+    </row>
+    <row r="546" spans="1:10">
+      <c r="A546" t="s">
+        <v>691</v>
+      </c>
+      <c r="B546" t="s">
+        <v>708</v>
+      </c>
+      <c r="C546">
+        <v>583594</v>
+      </c>
+      <c r="D546">
+        <v>1.580139</v>
+      </c>
+      <c r="E546">
+        <v>1.583126</v>
+      </c>
+      <c r="F546">
+        <v>1.58996</v>
+      </c>
+      <c r="G546">
+        <v>59.4</v>
+      </c>
+      <c r="H546">
+        <v>-2E-3</v>
+      </c>
+      <c r="J546" t="str">
+        <f t="shared" si="8"/>
+        <v>glasses.put("S-BAL42", new GlassMap("Ohara","S-BAL42",1.583126,1.580139,1.58996)); // 59.4 583594 -0.002</v>
+      </c>
+    </row>
+    <row r="547" spans="1:10">
+      <c r="A547" t="s">
+        <v>691</v>
+      </c>
+      <c r="B547" t="s">
+        <v>825</v>
+      </c>
+      <c r="C547">
+        <v>606437</v>
+      </c>
+      <c r="D547">
+        <v>1.601507</v>
+      </c>
+      <c r="E547">
+        <v>1.60562</v>
+      </c>
+      <c r="F547">
+        <v>1.615364</v>
+      </c>
+      <c r="G547">
+        <v>43.7</v>
+      </c>
+      <c r="H547">
+        <v>1.2999999999999999E-3</v>
+      </c>
+      <c r="J547" t="str">
+        <f t="shared" si="8"/>
+        <v>glasses.put("S-BAM4", new GlassMap("Ohara","S-BAM4",1.60562,1.601507,1.615364)); // 43.7 606437 0.0013</v>
+      </c>
+    </row>
+    <row r="548" spans="1:10">
+      <c r="A548" t="s">
+        <v>691</v>
+      </c>
+      <c r="B548" t="s">
+        <v>709</v>
+      </c>
+      <c r="C548">
+        <v>639449</v>
+      </c>
+      <c r="D548">
+        <v>1.635057</v>
+      </c>
+      <c r="E548">
+        <v>1.6393</v>
+      </c>
+      <c r="F548">
+        <v>1.6493040000000001</v>
+      </c>
+      <c r="G548">
+        <v>44.9</v>
+      </c>
+      <c r="H548">
+        <v>-5.9999999999999995E-4</v>
+      </c>
+      <c r="J548" t="str">
+        <f t="shared" si="8"/>
+        <v>glasses.put("S-BAM12", new GlassMap("Ohara","S-BAM12",1.6393,1.635057,1.649304)); // 44.9 639449 -0.0006</v>
+      </c>
+    </row>
+    <row r="549" spans="1:10">
+      <c r="A549" t="s">
+        <v>691</v>
+      </c>
+      <c r="B549" t="s">
+        <v>710</v>
+      </c>
+      <c r="C549">
+        <v>667483</v>
+      </c>
+      <c r="D549">
+        <v>1.6625890000000001</v>
+      </c>
+      <c r="E549">
+        <v>1.6667179999999999</v>
+      </c>
+      <c r="F549">
+        <v>1.6763859999999999</v>
+      </c>
+      <c r="G549">
+        <v>48.3</v>
+      </c>
+      <c r="H549">
+        <v>-2.3999999999999998E-3</v>
+      </c>
+      <c r="J549" t="str">
+        <f t="shared" si="8"/>
+        <v>glasses.put("S-BAH11", new GlassMap("Ohara","S-BAH11",1.666718,1.662589,1.676386)); // 48.3 667483 -0.0024</v>
+      </c>
+    </row>
+    <row r="550" spans="1:10">
+      <c r="A550" t="s">
+        <v>691</v>
+      </c>
+      <c r="B550" t="s">
+        <v>711</v>
+      </c>
+      <c r="C550">
+        <v>702412</v>
+      </c>
+      <c r="D550">
+        <v>1.6965030000000001</v>
+      </c>
+      <c r="E550">
+        <v>1.7015359999999999</v>
+      </c>
+      <c r="F550">
+        <v>1.7135149999999999</v>
+      </c>
+      <c r="G550">
+        <v>41.2</v>
+      </c>
+      <c r="H550">
+        <v>1.8E-3</v>
+      </c>
+      <c r="J550" t="str">
+        <f t="shared" si="8"/>
+        <v>glasses.put("S-BAH27", new GlassMap("Ohara","S-BAH27",1.701536,1.696503,1.713515)); // 41.2 702412 0.0018</v>
+      </c>
+    </row>
+    <row r="551" spans="1:10">
+      <c r="A551" t="s">
+        <v>691</v>
+      </c>
+      <c r="B551" t="s">
+        <v>712</v>
+      </c>
+      <c r="C551">
+        <v>723380</v>
+      </c>
+      <c r="D551">
+        <v>1.717816</v>
+      </c>
+      <c r="E551">
+        <v>1.72342</v>
+      </c>
+      <c r="F551">
+        <v>1.7368760000000001</v>
+      </c>
+      <c r="G551">
+        <v>38</v>
+      </c>
+      <c r="H551">
+        <v>3.5000000000000001E-3</v>
+      </c>
+      <c r="J551" t="str">
+        <f t="shared" si="8"/>
+        <v>glasses.put("S-BAH28", new GlassMap("Ohara","S-BAH28",1.72342,1.717816,1.736876)); // 38 723380 0.0035</v>
+      </c>
+    </row>
+    <row r="552" spans="1:10">
+      <c r="A552" t="s">
+        <v>691</v>
+      </c>
+      <c r="B552" t="s">
+        <v>713</v>
+      </c>
+      <c r="C552">
+        <v>618634</v>
+      </c>
+      <c r="D552">
+        <v>1.6150359999999999</v>
+      </c>
+      <c r="E552">
+        <v>1.6180000000000001</v>
+      </c>
+      <c r="F552">
+        <v>1.6247940000000001</v>
+      </c>
+      <c r="G552">
+        <v>63.4</v>
+      </c>
+      <c r="H552">
+        <v>5.1000000000000004E-3</v>
+      </c>
+      <c r="J552" t="str">
+        <f t="shared" si="8"/>
+        <v>glasses.put("S-PHM52", new GlassMap("Ohara","S-PHM52",1.618,1.615036,1.624794)); // 63.4 618634 0.0051</v>
+      </c>
+    </row>
+    <row r="553" spans="1:10">
+      <c r="A553" t="s">
+        <v>691</v>
+      </c>
+      <c r="B553" t="s">
+        <v>714</v>
+      </c>
+      <c r="C553">
+        <v>618633</v>
+      </c>
+      <c r="D553">
+        <v>1.615029</v>
+      </c>
+      <c r="E553">
+        <v>1.6180000000000001</v>
+      </c>
+      <c r="F553">
+        <v>1.624789</v>
+      </c>
+      <c r="G553">
+        <v>63.3</v>
+      </c>
+      <c r="H553">
+        <v>3.5999999999999999E-3</v>
+      </c>
+      <c r="J553" t="str">
+        <f t="shared" si="8"/>
+        <v>glasses.put("S-PHM52Q", new GlassMap("Ohara","S-PHM52Q",1.618,1.615029,1.624789)); // 63.3 618633 0.0036</v>
+      </c>
+    </row>
+    <row r="554" spans="1:10">
+      <c r="A554" t="s">
+        <v>691</v>
+      </c>
+      <c r="B554" t="s">
+        <v>715</v>
+      </c>
+      <c r="C554">
+        <v>603655</v>
+      </c>
+      <c r="D554">
+        <v>1.6001890000000001</v>
+      </c>
+      <c r="E554">
+        <v>1.6030009999999999</v>
+      </c>
+      <c r="F554">
+        <v>1.6094040000000001</v>
+      </c>
+      <c r="G554">
+        <v>65.5</v>
+      </c>
+      <c r="H554">
+        <v>4.4999999999999997E-3</v>
+      </c>
+      <c r="J554" t="str">
+        <f t="shared" si="8"/>
+        <v>glasses.put("S-PHM53", new GlassMap("Ohara","S-PHM53",1.603001,1.600189,1.609404)); // 65.5 603655 0.0045</v>
+      </c>
+    </row>
+    <row r="555" spans="1:10">
+      <c r="A555" t="s">
+        <v>691</v>
+      </c>
+      <c r="B555" t="s">
+        <v>800</v>
+      </c>
+      <c r="C555">
+        <v>548458</v>
+      </c>
+      <c r="D555">
+        <v>1.5445720000000001</v>
+      </c>
+      <c r="E555">
+        <v>1.548141</v>
+      </c>
+      <c r="F555">
+        <v>1.5565439999999999</v>
+      </c>
+      <c r="G555">
+        <v>45.8</v>
+      </c>
+      <c r="H555">
+        <v>1.1999999999999999E-3</v>
+      </c>
+      <c r="J555" t="str">
+        <f t="shared" si="8"/>
+        <v>glasses.put("S-TIL1", new GlassMap("Ohara","S-TIL1",1.548141,1.544572,1.556544)); // 45.8 548458 0.0012</v>
+      </c>
+    </row>
+    <row r="556" spans="1:10">
+      <c r="A556" t="s">
+        <v>691</v>
+      </c>
+      <c r="B556" t="s">
+        <v>801</v>
+      </c>
+      <c r="C556">
+        <v>541472</v>
+      </c>
+      <c r="D556">
+        <v>1.5372969999999999</v>
+      </c>
+      <c r="E556">
+        <v>1.5407200000000001</v>
+      </c>
+      <c r="F556">
+        <v>1.548746</v>
+      </c>
+      <c r="G556">
+        <v>47.2</v>
+      </c>
+      <c r="H556">
+        <v>0</v>
+      </c>
+      <c r="J556" t="str">
+        <f t="shared" si="8"/>
+        <v>glasses.put("S-TIL2", new GlassMap("Ohara","S-TIL2",1.54072,1.537297,1.548746)); // 47.2 541472 0</v>
+      </c>
+    </row>
+    <row r="557" spans="1:10">
+      <c r="A557" t="s">
+        <v>691</v>
+      </c>
+      <c r="B557" t="s">
+        <v>802</v>
+      </c>
+      <c r="C557">
+        <v>532489</v>
+      </c>
+      <c r="D557">
+        <v>1.528456</v>
+      </c>
+      <c r="E557">
+        <v>1.531717</v>
+      </c>
+      <c r="F557">
+        <v>1.5393429999999999</v>
+      </c>
+      <c r="G557">
+        <v>48.9</v>
+      </c>
+      <c r="H557">
+        <v>6.9999999999999999E-4</v>
+      </c>
+      <c r="J557" t="str">
+        <f t="shared" si="8"/>
+        <v>glasses.put("S-TIL6", new GlassMap("Ohara","S-TIL6",1.531717,1.528456,1.539343)); // 48.9 532489 0.0007</v>
+      </c>
+    </row>
+    <row r="558" spans="1:10">
+      <c r="A558" t="s">
+        <v>691</v>
+      </c>
+      <c r="B558" t="s">
+        <v>716</v>
+      </c>
+      <c r="C558">
+        <v>581407</v>
+      </c>
+      <c r="D558">
+        <v>1.577216</v>
+      </c>
+      <c r="E558">
+        <v>1.581439</v>
+      </c>
+      <c r="F558">
+        <v>1.591486</v>
+      </c>
+      <c r="G558">
+        <v>40.700000000000003</v>
+      </c>
+      <c r="H558">
+        <v>1.9E-3</v>
+      </c>
+      <c r="J558" t="str">
+        <f t="shared" si="8"/>
+        <v>glasses.put("S-TIL25", new GlassMap("Ohara","S-TIL25",1.581439,1.577216,1.591486)); // 40.7 581407 0.0019</v>
+      </c>
+    </row>
+    <row r="559" spans="1:10">
+      <c r="A559" t="s">
+        <v>691</v>
+      </c>
+      <c r="B559" t="s">
+        <v>717</v>
+      </c>
+      <c r="C559">
+        <v>567428</v>
+      </c>
+      <c r="D559">
+        <v>1.5633859999999999</v>
+      </c>
+      <c r="E559">
+        <v>1.5673220000000001</v>
+      </c>
+      <c r="F559">
+        <v>1.5766359999999999</v>
+      </c>
+      <c r="G559">
+        <v>42.8</v>
+      </c>
+      <c r="H559">
+        <v>8.9999999999999998E-4</v>
+      </c>
+      <c r="J559" t="str">
+        <f t="shared" si="8"/>
+        <v>glasses.put("S-TIL26", new GlassMap("Ohara","S-TIL26",1.567322,1.563386,1.576636)); // 42.8 567428 0.0009</v>
+      </c>
+    </row>
+    <row r="560" spans="1:10">
+      <c r="A560" t="s">
+        <v>691</v>
+      </c>
+      <c r="B560" t="s">
+        <v>718</v>
+      </c>
+      <c r="C560">
+        <v>575415</v>
+      </c>
+      <c r="D560">
+        <v>1.570902</v>
+      </c>
+      <c r="E560">
+        <v>1.5750059999999999</v>
+      </c>
+      <c r="F560">
+        <v>1.5847560000000001</v>
+      </c>
+      <c r="G560">
+        <v>41.5</v>
+      </c>
+      <c r="H560">
+        <v>2.3999999999999998E-3</v>
+      </c>
+      <c r="J560" t="str">
+        <f t="shared" si="8"/>
+        <v>glasses.put("S-TIL27", new GlassMap("Ohara","S-TIL27",1.575006,1.570902,1.584756)); // 41.5 575415 0.0024</v>
+      </c>
+    </row>
+    <row r="561" spans="1:10">
+      <c r="A561" t="s">
+        <v>691</v>
+      </c>
+      <c r="B561" t="s">
+        <v>803</v>
+      </c>
+      <c r="C561">
+        <v>620363</v>
+      </c>
+      <c r="D561">
+        <v>1.615024</v>
+      </c>
+      <c r="E561">
+        <v>1.6200410000000001</v>
+      </c>
+      <c r="F561">
+        <v>1.632123</v>
+      </c>
+      <c r="G561">
+        <v>36.299999999999997</v>
+      </c>
+      <c r="H561">
+        <v>5.1000000000000004E-3</v>
+      </c>
+      <c r="J561" t="str">
+        <f t="shared" si="8"/>
+        <v>glasses.put("S-TIM2", new GlassMap("Ohara","S-TIM2",1.620041,1.615024,1.632123)); // 36.3 620363 0.0051</v>
+      </c>
+    </row>
+    <row r="562" spans="1:10">
+      <c r="A562" t="s">
+        <v>691</v>
+      </c>
+      <c r="B562" t="s">
+        <v>804</v>
+      </c>
+      <c r="C562">
+        <v>603380</v>
+      </c>
+      <c r="D562">
+        <v>1.5987480000000001</v>
+      </c>
+      <c r="E562">
+        <v>1.6034200000000001</v>
+      </c>
+      <c r="F562">
+        <v>1.6146160000000001</v>
+      </c>
+      <c r="G562">
+        <v>38</v>
+      </c>
+      <c r="H562">
+        <v>3.5999999999999999E-3</v>
+      </c>
+      <c r="J562" t="str">
+        <f t="shared" si="8"/>
+        <v>glasses.put("S-TIM5", new GlassMap("Ohara","S-TIM5",1.60342,1.598748,1.614616)); // 38 603380 0.0036</v>
+      </c>
+    </row>
+    <row r="563" spans="1:10">
+      <c r="A563" t="s">
+        <v>691</v>
+      </c>
+      <c r="B563" t="s">
+        <v>805</v>
+      </c>
+      <c r="C563">
+        <v>596392</v>
+      </c>
+      <c r="D563">
+        <v>1.5910299999999999</v>
+      </c>
+      <c r="E563">
+        <v>1.5955090000000001</v>
+      </c>
+      <c r="F563">
+        <v>1.606206</v>
+      </c>
+      <c r="G563">
+        <v>39.200000000000003</v>
+      </c>
+      <c r="H563">
+        <v>2.3E-3</v>
+      </c>
+      <c r="J563" t="str">
+        <f t="shared" si="8"/>
+        <v>glasses.put("S-TIM8", new GlassMap("Ohara","S-TIM8",1.595509,1.59103,1.606206)); // 39.2 596392 0.0023</v>
+      </c>
+    </row>
+    <row r="564" spans="1:10">
+      <c r="A564" t="s">
+        <v>691</v>
+      </c>
+      <c r="B564" t="s">
+        <v>719</v>
+      </c>
+      <c r="C564">
+        <v>673321</v>
+      </c>
+      <c r="D564">
+        <v>1.6666069999999999</v>
+      </c>
+      <c r="E564">
+        <v>1.6727000000000001</v>
+      </c>
+      <c r="F564">
+        <v>1.6875640000000001</v>
+      </c>
+      <c r="G564">
+        <v>32.1</v>
+      </c>
+      <c r="H564">
+        <v>9.2999999999999992E-3</v>
+      </c>
+      <c r="J564" t="str">
+        <f t="shared" si="8"/>
+        <v>glasses.put("S-TIM25", new GlassMap("Ohara","S-TIM25",1.6727,1.666607,1.687564)); // 32.1 673321 0.0093</v>
+      </c>
+    </row>
+    <row r="565" spans="1:10">
+      <c r="A565" t="s">
+        <v>691</v>
+      </c>
+      <c r="B565" t="s">
+        <v>720</v>
+      </c>
+      <c r="C565">
+        <v>640345</v>
+      </c>
+      <c r="D565">
+        <v>1.6343749999999999</v>
+      </c>
+      <c r="E565">
+        <v>1.639799</v>
+      </c>
+      <c r="F565">
+        <v>1.6529389999999999</v>
+      </c>
+      <c r="G565">
+        <v>34.5</v>
+      </c>
+      <c r="H565">
+        <v>6.4999999999999997E-3</v>
+      </c>
+      <c r="J565" t="str">
+        <f t="shared" si="8"/>
+        <v>glasses.put("S-TIM27", new GlassMap("Ohara","S-TIM27",1.639799,1.634375,1.652939)); // 34.5 640345 0.0065</v>
+      </c>
+    </row>
+    <row r="566" spans="1:10">
+      <c r="A566" t="s">
+        <v>691</v>
+      </c>
+      <c r="B566" t="s">
+        <v>721</v>
+      </c>
+      <c r="C566">
+        <v>689311</v>
+      </c>
+      <c r="D566">
+        <v>1.6824950000000001</v>
+      </c>
+      <c r="E566">
+        <v>1.688931</v>
+      </c>
+      <c r="F566">
+        <v>1.7046650000000001</v>
+      </c>
+      <c r="G566">
+        <v>31.1</v>
+      </c>
+      <c r="H566">
+        <v>9.1999999999999998E-3</v>
+      </c>
+      <c r="J566" t="str">
+        <f t="shared" si="8"/>
+        <v>glasses.put("S-TIM28", new GlassMap("Ohara","S-TIM28",1.688931,1.682495,1.704665)); // 31.1 689311 0.0092</v>
+      </c>
+    </row>
+    <row r="567" spans="1:10">
+      <c r="A567" t="s">
+        <v>691</v>
+      </c>
+      <c r="B567" t="s">
+        <v>722</v>
+      </c>
+      <c r="C567">
+        <v>699301</v>
+      </c>
+      <c r="D567">
+        <v>1.6922250000000001</v>
+      </c>
+      <c r="E567">
+        <v>1.698947</v>
+      </c>
+      <c r="F567">
+        <v>1.7154240000000001</v>
+      </c>
+      <c r="G567">
+        <v>30.1</v>
+      </c>
+      <c r="H567">
+        <v>1.03E-2</v>
+      </c>
+      <c r="J567" t="str">
+        <f t="shared" si="8"/>
+        <v>glasses.put("S-TIM35", new GlassMap("Ohara","S-TIM35",1.698947,1.692225,1.715424)); // 30.1 699301 0.0103</v>
+      </c>
+    </row>
+    <row r="568" spans="1:10">
+      <c r="A568" t="s">
+        <v>691</v>
+      </c>
+      <c r="B568" t="s">
+        <v>806</v>
+      </c>
+      <c r="C568">
+        <v>717295</v>
+      </c>
+      <c r="D568">
+        <v>1.710332</v>
+      </c>
+      <c r="E568">
+        <v>1.7173620000000001</v>
+      </c>
+      <c r="F568">
+        <v>1.7346349999999999</v>
+      </c>
+      <c r="G568">
+        <v>29.5</v>
+      </c>
+      <c r="H568">
+        <v>1.0999999999999999E-2</v>
+      </c>
+      <c r="J568" t="str">
+        <f t="shared" si="8"/>
+        <v>glasses.put("S-TIH1", new GlassMap("Ohara","S-TIH1",1.717362,1.710332,1.734635)); // 29.5 717295 0.011</v>
+      </c>
+    </row>
+    <row r="569" spans="1:10">
+      <c r="A569" t="s">
+        <v>691</v>
+      </c>
+      <c r="B569" t="s">
+        <v>807</v>
+      </c>
+      <c r="C569">
+        <v>740283</v>
+      </c>
+      <c r="D569">
+        <v>1.732453</v>
+      </c>
+      <c r="E569">
+        <v>1.7399979999999999</v>
+      </c>
+      <c r="F569">
+        <v>1.758605</v>
+      </c>
+      <c r="G569">
+        <v>28.3</v>
+      </c>
+      <c r="H569">
+        <v>1.2200000000000001E-2</v>
+      </c>
+      <c r="J569" t="str">
+        <f t="shared" si="8"/>
+        <v>glasses.put("S-TIH3", new GlassMap("Ohara","S-TIH3",1.739998,1.732453,1.758605)); // 28.3 740283 0.0122</v>
+      </c>
+    </row>
+    <row r="570" spans="1:10">
+      <c r="A570" t="s">
+        <v>691</v>
+      </c>
+      <c r="B570" t="s">
+        <v>808</v>
+      </c>
+      <c r="C570">
+        <v>755275</v>
+      </c>
+      <c r="D570">
+        <v>1.747295</v>
+      </c>
+      <c r="E570">
+        <v>1.755199</v>
+      </c>
+      <c r="F570">
+        <v>1.774745</v>
+      </c>
+      <c r="G570">
+        <v>27.5</v>
+      </c>
+      <c r="H570">
+        <v>1.3299999999999999E-2</v>
+      </c>
+      <c r="J570" t="str">
+        <f t="shared" si="8"/>
+        <v>glasses.put("S-TIH4", new GlassMap("Ohara","S-TIH4",1.755199,1.747295,1.774745)); // 27.5 755275 0.0133</v>
+      </c>
+    </row>
+    <row r="571" spans="1:10">
+      <c r="A571" t="s">
+        <v>691</v>
+      </c>
+      <c r="B571" t="s">
+        <v>809</v>
+      </c>
+      <c r="C571">
+        <v>805254</v>
+      </c>
+      <c r="D571">
+        <v>1.796106</v>
+      </c>
+      <c r="E571">
+        <v>1.8051809999999999</v>
+      </c>
+      <c r="F571">
+        <v>1.8277749999999999</v>
+      </c>
+      <c r="G571">
+        <v>25.4</v>
+      </c>
+      <c r="H571">
+        <v>1.5800000000000002E-2</v>
+      </c>
+      <c r="J571" t="str">
+        <f t="shared" si="8"/>
+        <v>glasses.put("S-TIH6", new GlassMap("Ohara","S-TIH6",1.805181,1.796106,1.827775)); // 25.4 805254 0.0158</v>
+      </c>
+    </row>
+    <row r="572" spans="1:10">
+      <c r="A572" t="s">
+        <v>691</v>
+      </c>
+      <c r="B572" t="s">
+        <v>723</v>
+      </c>
+      <c r="C572">
+        <v>728285</v>
+      </c>
+      <c r="D572">
+        <v>1.7208650000000001</v>
+      </c>
+      <c r="E572">
+        <v>1.7282500000000001</v>
+      </c>
+      <c r="F572">
+        <v>1.746453</v>
+      </c>
+      <c r="G572">
+        <v>28.5</v>
+      </c>
+      <c r="H572">
+        <v>1.23E-2</v>
+      </c>
+      <c r="J572" t="str">
+        <f t="shared" si="8"/>
+        <v>glasses.put("S-TIH10", new GlassMap("Ohara","S-TIH10",1.72825,1.720865,1.746453)); // 28.5 728285 0.0123</v>
+      </c>
+    </row>
+    <row r="573" spans="1:10">
+      <c r="A573" t="s">
+        <v>691</v>
+      </c>
+      <c r="B573" t="s">
+        <v>724</v>
+      </c>
+      <c r="C573">
+        <v>785257</v>
+      </c>
+      <c r="D573">
+        <v>1.775965</v>
+      </c>
+      <c r="E573">
+        <v>1.7847230000000001</v>
+      </c>
+      <c r="F573">
+        <v>1.806519</v>
+      </c>
+      <c r="G573">
+        <v>25.7</v>
+      </c>
+      <c r="H573">
+        <v>1.6199999999999999E-2</v>
+      </c>
+      <c r="J573" t="str">
+        <f t="shared" si="8"/>
+        <v>glasses.put("S-TIH11", new GlassMap("Ohara","S-TIH11",1.784723,1.775965,1.806519)); // 25.7 785257 0.0162</v>
+      </c>
+    </row>
+    <row r="574" spans="1:10">
+      <c r="A574" t="s">
+        <v>691</v>
+      </c>
+      <c r="B574" t="s">
+        <v>725</v>
+      </c>
+      <c r="C574">
+        <v>741278</v>
+      </c>
+      <c r="D574">
+        <v>1.7330890000000001</v>
+      </c>
+      <c r="E574">
+        <v>1.740769</v>
+      </c>
+      <c r="F574">
+        <v>1.759746</v>
+      </c>
+      <c r="G574">
+        <v>27.8</v>
+      </c>
+      <c r="H574">
+        <v>1.2999999999999999E-2</v>
+      </c>
+      <c r="J574" t="str">
+        <f t="shared" si="8"/>
+        <v>glasses.put("S-TIH13", new GlassMap("Ohara","S-TIH13",1.740769,1.733089,1.759746)); // 27.8 741278 0.013</v>
+      </c>
+    </row>
+    <row r="575" spans="1:10">
+      <c r="A575" t="s">
+        <v>691</v>
+      </c>
+      <c r="B575" t="s">
+        <v>726</v>
+      </c>
+      <c r="C575">
+        <v>762265</v>
+      </c>
+      <c r="D575">
+        <v>1.7535670000000001</v>
+      </c>
+      <c r="E575">
+        <v>1.7618210000000001</v>
+      </c>
+      <c r="F575">
+        <v>1.7822960000000001</v>
+      </c>
+      <c r="G575">
+        <v>26.5</v>
+      </c>
+      <c r="H575">
+        <v>1.4999999999999999E-2</v>
+      </c>
+      <c r="J575" t="str">
+        <f t="shared" si="8"/>
+        <v>glasses.put("S-TIH14", new GlassMap("Ohara","S-TIH14",1.761821,1.753567,1.782296)); // 26.5 762265 0.015</v>
+      </c>
+    </row>
+    <row r="576" spans="1:10">
+      <c r="A576" t="s">
+        <v>691</v>
+      </c>
+      <c r="B576" t="s">
+        <v>727</v>
+      </c>
+      <c r="C576">
+        <v>722292</v>
+      </c>
+      <c r="D576">
+        <v>1.7143710000000001</v>
+      </c>
+      <c r="E576">
+        <v>1.7215069999999999</v>
+      </c>
+      <c r="F576">
+        <v>1.7390540000000001</v>
+      </c>
+      <c r="G576">
+        <v>29.2</v>
+      </c>
+      <c r="H576">
+        <v>1.11E-2</v>
+      </c>
+      <c r="J576" t="str">
+        <f t="shared" si="8"/>
+        <v>glasses.put("S-TIH18", new GlassMap("Ohara","S-TIH18",1.721507,1.714371,1.739054)); // 29.2 722292 0.0111</v>
+      </c>
+    </row>
+    <row r="577" spans="1:10">
+      <c r="A577" t="s">
+        <v>691</v>
+      </c>
+      <c r="B577" t="s">
+        <v>728</v>
+      </c>
+      <c r="C577">
+        <v>847238</v>
+      </c>
+      <c r="D577">
+        <v>1.8364879999999999</v>
+      </c>
+      <c r="E577">
+        <v>1.84666</v>
+      </c>
+      <c r="F577">
+        <v>1.872096</v>
+      </c>
+      <c r="G577">
+        <v>23.8</v>
+      </c>
+      <c r="H577">
+        <v>1.7500000000000002E-2</v>
+      </c>
+      <c r="J577" t="str">
+        <f t="shared" si="8"/>
+        <v>glasses.put("S-TIH53", new GlassMap("Ohara","S-TIH53",1.84666,1.836488,1.872096)); // 23.8 847238 0.0175</v>
+      </c>
+    </row>
+    <row r="578" spans="1:10">
+      <c r="A578" t="s">
+        <v>691</v>
+      </c>
+      <c r="B578" t="s">
+        <v>729</v>
+      </c>
+      <c r="C578">
+        <v>847238</v>
+      </c>
+      <c r="D578">
+        <v>1.8364879999999999</v>
+      </c>
+      <c r="E578">
+        <v>1.84666</v>
+      </c>
+      <c r="F578">
+        <v>1.872096</v>
+      </c>
+      <c r="G578">
+        <v>23.8</v>
+      </c>
+      <c r="H578">
+        <v>1.7500000000000002E-2</v>
+      </c>
+      <c r="J578" t="str">
+        <f t="shared" si="8"/>
+        <v>glasses.put("S-TIH53W", new GlassMap("Ohara","S-TIH53W",1.84666,1.836488,1.872096)); // 23.8 847238 0.0175</v>
+      </c>
+    </row>
+    <row r="579" spans="1:10">
+      <c r="A579" t="s">
+        <v>691</v>
+      </c>
+      <c r="B579" t="s">
+        <v>730</v>
+      </c>
+      <c r="C579">
+        <v>847239</v>
+      </c>
+      <c r="D579">
+        <v>1.836527</v>
+      </c>
+      <c r="E579">
+        <v>1.84666</v>
+      </c>
+      <c r="F579">
+        <v>1.872007</v>
+      </c>
+      <c r="G579">
+        <v>23.9</v>
+      </c>
+      <c r="H579">
+        <v>1.7899999999999999E-2</v>
+      </c>
+      <c r="J579" t="str">
+        <f t="shared" ref="J579:J642" si="9">CONCATENATE("glasses.put(""",B579,""", new GlassMap(""",A579,""",""",B579,""",",E579,",",D579,",",F579,")); // ",G579, " ",C579," ",H579)</f>
+        <v>glasses.put("S-TIH53WN", new GlassMap("Ohara","S-TIH53WN",1.84666,1.836527,1.872007)); // 23.9 847239 0.0179</v>
+      </c>
+    </row>
+    <row r="580" spans="1:10">
+      <c r="A580" t="s">
+        <v>691</v>
+      </c>
+      <c r="B580" t="s">
+        <v>731</v>
+      </c>
+      <c r="C580">
+        <v>963241</v>
+      </c>
+      <c r="D580">
+        <v>1.9515979999999999</v>
+      </c>
+      <c r="E580">
+        <v>1.9630000000000001</v>
+      </c>
+      <c r="F580">
+        <v>1.991533</v>
+      </c>
+      <c r="G580">
+        <v>24.1</v>
+      </c>
+      <c r="H580">
+        <v>1.8700000000000001E-2</v>
+      </c>
+      <c r="J580" t="str">
+        <f t="shared" si="9"/>
+        <v>glasses.put("S-TIH57", new GlassMap("Ohara","S-TIH57",1.963,1.951598,1.991533)); // 24.1 963241 0.0187</v>
+      </c>
+    </row>
+    <row r="581" spans="1:10">
+      <c r="A581" t="s">
+        <v>691</v>
+      </c>
+      <c r="B581" t="s">
+        <v>810</v>
+      </c>
+      <c r="C581">
+        <v>652585</v>
+      </c>
+      <c r="D581">
+        <v>1.6481920000000001</v>
+      </c>
+      <c r="E581">
+        <v>1.6516</v>
+      </c>
+      <c r="F581">
+        <v>1.659322</v>
+      </c>
+      <c r="G581">
+        <v>58.5</v>
+      </c>
+      <c r="H581">
+        <v>-7.7999999999999996E-3</v>
+      </c>
+      <c r="J581" t="str">
+        <f t="shared" si="9"/>
+        <v>glasses.put("S-LAL7Q", new GlassMap("Ohara","S-LAL7Q",1.6516,1.648192,1.659322)); // 58.5 652585 -0.0078</v>
+      </c>
+    </row>
+    <row r="582" spans="1:10">
+      <c r="A582" t="s">
+        <v>691</v>
+      </c>
+      <c r="B582" t="s">
+        <v>811</v>
+      </c>
+      <c r="C582">
+        <v>713539</v>
+      </c>
+      <c r="D582">
+        <v>1.708974</v>
+      </c>
+      <c r="E582">
+        <v>1.712995</v>
+      </c>
+      <c r="F582">
+        <v>1.72221</v>
+      </c>
+      <c r="G582">
+        <v>53.9</v>
+      </c>
+      <c r="H582">
+        <v>-8.3999999999999995E-3</v>
+      </c>
+      <c r="J582" t="str">
+        <f t="shared" si="9"/>
+        <v>glasses.put("S-LAL8", new GlassMap("Ohara","S-LAL8",1.712995,1.708974,1.72221)); // 53.9 713539 -0.0084</v>
+      </c>
+    </row>
+    <row r="583" spans="1:10">
+      <c r="A583" t="s">
+        <v>691</v>
+      </c>
+      <c r="B583" t="s">
+        <v>812</v>
+      </c>
+      <c r="C583">
+        <v>691548</v>
+      </c>
+      <c r="D583">
+        <v>1.6871689999999999</v>
+      </c>
+      <c r="E583">
+        <v>1.6910019999999999</v>
+      </c>
+      <c r="F583">
+        <v>1.6997739999999999</v>
+      </c>
+      <c r="G583">
+        <v>54.8</v>
+      </c>
+      <c r="H583">
+        <v>-7.9000000000000008E-3</v>
+      </c>
+      <c r="J583" t="str">
+        <f t="shared" si="9"/>
+        <v>glasses.put("S-LAL9", new GlassMap("Ohara","S-LAL9",1.691002,1.687169,1.699774)); // 54.8 691548 -0.0079</v>
+      </c>
+    </row>
+    <row r="584" spans="1:10">
+      <c r="A584" t="s">
+        <v>691</v>
+      </c>
+      <c r="B584" t="s">
+        <v>732</v>
+      </c>
+      <c r="C584">
+        <v>720502</v>
+      </c>
+      <c r="D584">
+        <v>1.71567</v>
+      </c>
+      <c r="E584">
+        <v>1.7199949999999999</v>
+      </c>
+      <c r="F584">
+        <v>1.7300040000000001</v>
+      </c>
+      <c r="G584">
+        <v>50.2</v>
+      </c>
+      <c r="H584">
+        <v>-8.0999999999999996E-3</v>
+      </c>
+      <c r="J584" t="str">
+        <f t="shared" si="9"/>
+        <v>glasses.put("S-LAL10", new GlassMap("Ohara","S-LAL10",1.719995,1.71567,1.730004)); // 50.2 720502 -0.0081</v>
+      </c>
+    </row>
+    <row r="585" spans="1:10">
+      <c r="A585" t="s">
+        <v>691</v>
+      </c>
+      <c r="B585" t="s">
+        <v>733</v>
+      </c>
+      <c r="C585">
+        <v>678553</v>
+      </c>
+      <c r="D585">
+        <v>1.674188</v>
+      </c>
+      <c r="E585">
+        <v>1.6778999999999999</v>
+      </c>
+      <c r="F585">
+        <v>1.6864380000000001</v>
+      </c>
+      <c r="G585">
+        <v>55.3</v>
+      </c>
+      <c r="H585">
+        <v>-4.7000000000000002E-3</v>
+      </c>
+      <c r="J585" t="str">
+        <f t="shared" si="9"/>
+        <v>glasses.put("S-LAL12", new GlassMap("Ohara","S-LAL12",1.6779,1.674188,1.686438)); // 55.3 678553 -0.0047</v>
+      </c>
+    </row>
+    <row r="586" spans="1:10">
+      <c r="A586" t="s">
+        <v>691</v>
+      </c>
+      <c r="B586" t="s">
+        <v>734</v>
+      </c>
+      <c r="C586">
+        <v>678553</v>
+      </c>
+      <c r="D586">
+        <v>1.6741710000000001</v>
+      </c>
+      <c r="E586">
+        <v>1.6778999999999999</v>
+      </c>
+      <c r="F586">
+        <v>1.6864189999999999</v>
+      </c>
+      <c r="G586">
+        <v>55.3</v>
+      </c>
+      <c r="H586">
+        <v>-8.5000000000000006E-3</v>
+      </c>
+      <c r="J586" t="str">
+        <f t="shared" si="9"/>
+        <v>glasses.put("S-LAL12Q", new GlassMap("Ohara","S-LAL12Q",1.6779,1.674171,1.686419)); // 55.3 678553 -0.0085</v>
+      </c>
+    </row>
+    <row r="587" spans="1:10">
+      <c r="A587" t="s">
+        <v>691</v>
+      </c>
+      <c r="B587" t="s">
+        <v>735</v>
+      </c>
+      <c r="C587">
+        <v>697555</v>
+      </c>
+      <c r="D587">
+        <v>1.692974</v>
+      </c>
+      <c r="E587">
+        <v>1.6967970000000001</v>
+      </c>
+      <c r="F587">
+        <v>1.705522</v>
+      </c>
+      <c r="G587">
+        <v>55.5</v>
+      </c>
+      <c r="H587">
+        <v>-8.2000000000000007E-3</v>
+      </c>
+      <c r="J587" t="str">
+        <f t="shared" si="9"/>
+        <v>glasses.put("S-LAL14", new GlassMap("Ohara","S-LAL14",1.696797,1.692974,1.705522)); // 55.5 697555 -0.0082</v>
+      </c>
+    </row>
+    <row r="588" spans="1:10">
+      <c r="A588" t="s">
+        <v>691</v>
+      </c>
+      <c r="B588" t="s">
+        <v>736</v>
+      </c>
+      <c r="C588">
+        <v>729547</v>
+      </c>
+      <c r="D588">
+        <v>1.725101</v>
+      </c>
+      <c r="E588">
+        <v>1.7291570000000001</v>
+      </c>
+      <c r="F588">
+        <v>1.7384360000000001</v>
+      </c>
+      <c r="G588">
+        <v>54.7</v>
+      </c>
+      <c r="H588">
+        <v>-8.6E-3</v>
+      </c>
+      <c r="J588" t="str">
+        <f t="shared" si="9"/>
+        <v>glasses.put("S-LAL18", new GlassMap("Ohara","S-LAL18",1.729157,1.725101,1.738436)); // 54.7 729547 -0.0086</v>
+      </c>
+    </row>
+    <row r="589" spans="1:10">
+      <c r="A589" t="s">
+        <v>691</v>
+      </c>
+      <c r="B589" t="s">
+        <v>737</v>
+      </c>
+      <c r="C589">
+        <v>729546</v>
+      </c>
+      <c r="D589">
+        <v>1.725093</v>
+      </c>
+      <c r="E589">
+        <v>1.7291570000000001</v>
+      </c>
+      <c r="F589">
+        <v>1.7384489999999999</v>
+      </c>
+      <c r="G589">
+        <v>54.6</v>
+      </c>
+      <c r="H589">
+        <v>-8.8999999999999999E-3</v>
+      </c>
+      <c r="J589" t="str">
+        <f t="shared" si="9"/>
+        <v>glasses.put("S-LAL18N", new GlassMap("Ohara","S-LAL18N",1.729157,1.725093,1.738449)); // 54.6 729546 -0.0089</v>
+      </c>
+    </row>
+    <row r="590" spans="1:10">
+      <c r="A590" t="s">
+        <v>691</v>
+      </c>
+      <c r="B590" t="s">
+        <v>738</v>
+      </c>
+      <c r="C590">
+        <v>729541</v>
+      </c>
+      <c r="D590">
+        <v>1.725061</v>
+      </c>
+      <c r="E590">
+        <v>1.72916</v>
+      </c>
+      <c r="F590">
+        <v>1.7385409999999999</v>
+      </c>
+      <c r="G590">
+        <v>54.1</v>
+      </c>
+      <c r="H590">
+        <v>-9.1999999999999998E-3</v>
+      </c>
+      <c r="J590" t="str">
+        <f t="shared" si="9"/>
+        <v>glasses.put("S-LAL19", new GlassMap("Ohara","S-LAL19",1.72916,1.725061,1.738541)); // 54.1 729541 -0.0092</v>
+      </c>
+    </row>
+    <row r="591" spans="1:10">
+      <c r="A591" t="s">
+        <v>691</v>
+      </c>
+      <c r="B591" t="s">
+        <v>739</v>
+      </c>
+      <c r="C591">
+        <v>699511</v>
+      </c>
+      <c r="D591">
+        <v>1.6951959999999999</v>
+      </c>
+      <c r="E591">
+        <v>1.6993</v>
+      </c>
+      <c r="F591">
+        <v>1.7088779999999999</v>
+      </c>
+      <c r="G591">
+        <v>51.1</v>
+      </c>
+      <c r="H591">
+        <v>-3.5999999999999999E-3</v>
+      </c>
+      <c r="J591" t="str">
+        <f t="shared" si="9"/>
+        <v>glasses.put("S-LAL20", new GlassMap("Ohara","S-LAL20",1.6993,1.695196,1.708878)); // 51.1 699511 -0.0036</v>
+      </c>
+    </row>
+    <row r="592" spans="1:10">
+      <c r="A592" t="s">
+        <v>691</v>
+      </c>
+      <c r="B592" t="s">
+        <v>740</v>
+      </c>
+      <c r="C592">
+        <v>703524</v>
+      </c>
+      <c r="D592">
+        <v>1.698952</v>
+      </c>
+      <c r="E592">
+        <v>1.7030000000000001</v>
+      </c>
+      <c r="F592">
+        <v>1.7123740000000001</v>
+      </c>
+      <c r="G592">
+        <v>52.4</v>
+      </c>
+      <c r="H592">
+        <v>-6.1000000000000004E-3</v>
+      </c>
+      <c r="J592" t="str">
+        <f t="shared" si="9"/>
+        <v>glasses.put("S-LAL21", new GlassMap("Ohara","S-LAL21",1.703,1.698952,1.712374)); // 52.4 703524 -0.0061</v>
+      </c>
+    </row>
+    <row r="593" spans="1:10">
+      <c r="A593" t="s">
+        <v>691</v>
+      </c>
+      <c r="B593" t="s">
+        <v>741</v>
+      </c>
+      <c r="C593">
+        <v>651562</v>
+      </c>
+      <c r="D593">
+        <v>1.64747</v>
+      </c>
+      <c r="E593">
+        <v>1.651</v>
+      </c>
+      <c r="F593">
+        <v>1.659046</v>
+      </c>
+      <c r="G593">
+        <v>56.2</v>
+      </c>
+      <c r="H593">
+        <v>-8.5000000000000006E-3</v>
+      </c>
+      <c r="J593" t="str">
+        <f t="shared" si="9"/>
+        <v>glasses.put("S-LAL54Q", new GlassMap("Ohara","S-LAL54Q",1.651,1.64747,1.659046)); // 56.2 651562 -0.0085</v>
+      </c>
+    </row>
+    <row r="594" spans="1:10">
+      <c r="A594" t="s">
+        <v>691</v>
+      </c>
+      <c r="B594" t="s">
+        <v>742</v>
+      </c>
+      <c r="C594">
+        <v>694508</v>
+      </c>
+      <c r="D594">
+        <v>1.6893929999999999</v>
+      </c>
+      <c r="E594">
+        <v>1.693495</v>
+      </c>
+      <c r="F594">
+        <v>1.7030419999999999</v>
+      </c>
+      <c r="G594">
+        <v>50.8</v>
+      </c>
+      <c r="H594">
+        <v>-4.7000000000000002E-3</v>
+      </c>
+      <c r="J594" t="str">
+        <f t="shared" si="9"/>
+        <v>glasses.put("S-LAL58", new GlassMap("Ohara","S-LAL58",1.693495,1.689393,1.703042)); // 50.8 694508 -0.0047</v>
+      </c>
+    </row>
+    <row r="595" spans="1:10">
+      <c r="A595" t="s">
+        <v>691</v>
+      </c>
+      <c r="B595" t="s">
+        <v>743</v>
+      </c>
+      <c r="C595">
+        <v>734515</v>
+      </c>
+      <c r="D595">
+        <v>1.729679</v>
+      </c>
+      <c r="E595">
+        <v>1.733997</v>
+      </c>
+      <c r="F595">
+        <v>1.74394</v>
+      </c>
+      <c r="G595">
+        <v>51.5</v>
+      </c>
+      <c r="H595">
+        <v>-9.5999999999999992E-3</v>
+      </c>
+      <c r="J595" t="str">
+        <f t="shared" si="9"/>
+        <v>glasses.put("S-LAL59", new GlassMap("Ohara","S-LAL59",1.733997,1.729679,1.74394)); // 51.5 734515 -0.0096</v>
+      </c>
+    </row>
+    <row r="596" spans="1:10">
+      <c r="A596" t="s">
+        <v>691</v>
+      </c>
+      <c r="B596" t="s">
+        <v>744</v>
+      </c>
+      <c r="C596">
+        <v>741527</v>
+      </c>
+      <c r="D596">
+        <v>1.7367269999999999</v>
+      </c>
+      <c r="E596">
+        <v>1.740999</v>
+      </c>
+      <c r="F596">
+        <v>1.7508049999999999</v>
+      </c>
+      <c r="G596">
+        <v>52.7</v>
+      </c>
+      <c r="H596">
+        <v>-9.5999999999999992E-3</v>
+      </c>
+      <c r="J596" t="str">
+        <f t="shared" si="9"/>
+        <v>glasses.put("S-LAL61", new GlassMap("Ohara","S-LAL61",1.740999,1.736727,1.750805)); // 52.7 741527 -0.0096</v>
+      </c>
+    </row>
+    <row r="597" spans="1:10">
+      <c r="A597" t="s">
+        <v>691</v>
+      </c>
+      <c r="B597" t="s">
+        <v>745</v>
+      </c>
+      <c r="C597">
+        <v>741526</v>
+      </c>
+      <c r="D597">
+        <v>1.7367330000000001</v>
+      </c>
+      <c r="E597">
+        <v>1.7410000000000001</v>
+      </c>
+      <c r="F597">
+        <v>1.75082</v>
+      </c>
+      <c r="G597">
+        <v>52.6</v>
+      </c>
+      <c r="H597">
+        <v>-8.5000000000000006E-3</v>
+      </c>
+      <c r="J597" t="str">
+        <f t="shared" si="9"/>
+        <v>glasses.put("S-LAL61Q", new GlassMap("Ohara","S-LAL61Q",1.741,1.736733,1.75082)); // 52.6 741526 -0.0085</v>
+      </c>
+    </row>
+    <row r="598" spans="1:10">
+      <c r="A598" t="s">
+        <v>691</v>
+      </c>
+      <c r="B598" t="s">
+        <v>822</v>
+      </c>
+      <c r="C598">
+        <v>744448</v>
+      </c>
+      <c r="D598">
+        <v>1.7390479999999999</v>
+      </c>
+      <c r="E598">
+        <v>1.743997</v>
+      </c>
+      <c r="F598">
+        <v>1.7556609999999999</v>
+      </c>
+      <c r="G598">
+        <v>44.8</v>
+      </c>
+      <c r="H598">
+        <v>-3.5000000000000001E-3</v>
+      </c>
+      <c r="J598" t="str">
+        <f t="shared" si="9"/>
+        <v>glasses.put("S-LAM2", new GlassMap("Ohara","S-LAM2",1.743997,1.739048,1.755661)); // 44.8 744448 -0.0035</v>
+      </c>
+    </row>
+    <row r="599" spans="1:10">
+      <c r="A599" t="s">
+        <v>691</v>
+      </c>
+      <c r="B599" t="s">
+        <v>823</v>
+      </c>
+      <c r="C599">
+        <v>717479</v>
+      </c>
+      <c r="D599">
+        <v>1.7125280000000001</v>
+      </c>
+      <c r="E599">
+        <v>1.717004</v>
+      </c>
+      <c r="F599">
+        <v>1.7274890000000001</v>
+      </c>
+      <c r="G599">
+        <v>47.9</v>
+      </c>
+      <c r="H599">
+        <v>-3.3999999999999998E-3</v>
+      </c>
+      <c r="J599" t="str">
+        <f t="shared" si="9"/>
+        <v>glasses.put("S-LAM3", new GlassMap("Ohara","S-LAM3",1.717004,1.712528,1.727489)); // 47.9 717479 -0.0034</v>
+      </c>
+    </row>
+    <row r="600" spans="1:10">
+      <c r="A600" t="s">
+        <v>691</v>
+      </c>
+      <c r="B600" t="s">
+        <v>824</v>
+      </c>
+      <c r="C600">
+        <v>750353</v>
+      </c>
+      <c r="D600">
+        <v>1.7432749999999999</v>
+      </c>
+      <c r="E600">
+        <v>1.7494970000000001</v>
+      </c>
+      <c r="F600">
+        <v>1.764518</v>
+      </c>
+      <c r="G600">
+        <v>35.299999999999997</v>
+      </c>
+      <c r="H600">
+        <v>2.5000000000000001E-3</v>
+      </c>
+      <c r="J600" t="str">
+        <f t="shared" si="9"/>
+        <v>glasses.put("S-LAM7", new GlassMap("Ohara","S-LAM7",1.749497,1.743275,1.764518)); // 35.3 750353 0.0025</v>
+      </c>
+    </row>
+    <row r="601" spans="1:10">
+      <c r="A601" t="s">
+        <v>691</v>
+      </c>
+      <c r="B601" t="s">
+        <v>746</v>
+      </c>
+      <c r="C601">
+        <v>762401</v>
+      </c>
+      <c r="D601">
+        <v>1.7563850000000001</v>
+      </c>
+      <c r="E601">
+        <v>1.7620009999999999</v>
+      </c>
+      <c r="F601">
+        <v>1.775388</v>
+      </c>
+      <c r="G601">
+        <v>40.1</v>
+      </c>
+      <c r="H601">
+        <v>-1E-4</v>
+      </c>
+      <c r="J601" t="str">
+        <f t="shared" si="9"/>
+        <v>glasses.put("S-LAM55", new GlassMap("Ohara","S-LAM55",1.762001,1.756385,1.775388)); // 40.1 762401 -0.0001</v>
+      </c>
+    </row>
+    <row r="602" spans="1:10">
+      <c r="A602" t="s">
+        <v>691</v>
+      </c>
+      <c r="B602" t="s">
+        <v>747</v>
+      </c>
+      <c r="C602">
+        <v>743493</v>
+      </c>
+      <c r="D602">
+        <v>1.738653</v>
+      </c>
+      <c r="E602">
+        <v>1.743198</v>
+      </c>
+      <c r="F602">
+        <v>1.7537160000000001</v>
+      </c>
+      <c r="G602">
+        <v>49.3</v>
+      </c>
+      <c r="H602">
+        <v>-8.5000000000000006E-3</v>
+      </c>
+      <c r="J602" t="str">
+        <f t="shared" si="9"/>
+        <v>glasses.put("S-LAM60", new GlassMap("Ohara","S-LAM60",1.743198,1.738653,1.753716)); // 49.3 743493 -0.0085</v>
+      </c>
+    </row>
+    <row r="603" spans="1:10">
+      <c r="A603" t="s">
+        <v>691</v>
+      </c>
+      <c r="B603" t="s">
+        <v>748</v>
+      </c>
+      <c r="C603">
+        <v>801350</v>
+      </c>
+      <c r="D603">
+        <v>1.7942750000000001</v>
+      </c>
+      <c r="E603">
+        <v>1.800999</v>
+      </c>
+      <c r="F603">
+        <v>1.8171820000000001</v>
+      </c>
+      <c r="G603">
+        <v>35</v>
+      </c>
+      <c r="H603">
+        <v>1.5E-3</v>
+      </c>
+      <c r="J603" t="str">
+        <f t="shared" si="9"/>
+        <v>glasses.put("S-LAM66", new GlassMap("Ohara","S-LAM66",1.800999,1.794275,1.817182)); // 35 801350 0.0015</v>
+      </c>
+    </row>
+    <row r="604" spans="1:10">
+      <c r="A604" t="s">
+        <v>691</v>
+      </c>
+      <c r="B604" t="s">
+        <v>749</v>
+      </c>
+      <c r="C604">
+        <v>794371</v>
+      </c>
+      <c r="D604">
+        <v>1.7873190000000001</v>
+      </c>
+      <c r="E604">
+        <v>1.7936000000000001</v>
+      </c>
+      <c r="F604">
+        <v>1.808716</v>
+      </c>
+      <c r="G604">
+        <v>37.1</v>
+      </c>
+      <c r="H604">
+        <v>1.2999999999999999E-3</v>
+      </c>
+      <c r="J604" t="str">
+        <f t="shared" si="9"/>
+        <v>glasses.put("S-LAM73", new GlassMap("Ohara","S-LAM73",1.7936,1.787319,1.808716)); // 37.1 794371 0.0013</v>
+      </c>
+    </row>
+    <row r="605" spans="1:10">
+      <c r="A605" t="s">
+        <v>691</v>
+      </c>
+      <c r="B605" t="s">
+        <v>750</v>
+      </c>
+      <c r="C605">
+        <v>786442</v>
+      </c>
+      <c r="D605">
+        <v>1.7805839999999999</v>
+      </c>
+      <c r="E605">
+        <v>1.7858959999999999</v>
+      </c>
+      <c r="F605">
+        <v>1.7983640000000001</v>
+      </c>
+      <c r="G605">
+        <v>44.2</v>
+      </c>
+      <c r="H605">
+        <v>-6.8999999999999999E-3</v>
+      </c>
+      <c r="J605" t="str">
+        <f t="shared" si="9"/>
+        <v>glasses.put("S-LAH51", new GlassMap("Ohara","S-LAH51",1.785896,1.780584,1.798364)); // 44.2 786442 -0.0069</v>
+      </c>
+    </row>
+    <row r="606" spans="1:10">
+      <c r="A606" t="s">
+        <v>691</v>
+      </c>
+      <c r="B606" t="s">
+        <v>751</v>
+      </c>
+      <c r="C606">
+        <v>800422</v>
+      </c>
+      <c r="D606">
+        <v>1.793879</v>
+      </c>
+      <c r="E606">
+        <v>1.7995159999999999</v>
+      </c>
+      <c r="F606">
+        <v>1.8128139999999999</v>
+      </c>
+      <c r="G606">
+        <v>42.2</v>
+      </c>
+      <c r="H606">
+        <v>-6.0000000000000001E-3</v>
+      </c>
+      <c r="J606" t="str">
+        <f t="shared" si="9"/>
+        <v>glasses.put("S-LAH52", new GlassMap("Ohara","S-LAH52",1.799516,1.793879,1.812814)); // 42.2 800422 -0.006</v>
+      </c>
+    </row>
+    <row r="607" spans="1:10">
+      <c r="A607" t="s">
+        <v>691</v>
+      </c>
+      <c r="B607" t="s">
+        <v>752</v>
+      </c>
+      <c r="C607">
+        <v>800422</v>
+      </c>
+      <c r="D607">
+        <v>1.793893</v>
+      </c>
+      <c r="E607">
+        <v>1.79952</v>
+      </c>
+      <c r="F607">
+        <v>1.812821</v>
+      </c>
+      <c r="G607">
+        <v>42.2</v>
+      </c>
+      <c r="H607">
+        <v>-5.5999999999999999E-3</v>
+      </c>
+      <c r="J607" t="str">
+        <f t="shared" si="9"/>
+        <v>glasses.put("S-LAH52Q", new GlassMap("Ohara","S-LAH52Q",1.79952,1.793893,1.812821)); // 42.2 800422 -0.0056</v>
+      </c>
+    </row>
+    <row r="608" spans="1:10">
+      <c r="A608" t="s">
+        <v>691</v>
+      </c>
+      <c r="B608" t="s">
+        <v>753</v>
+      </c>
+      <c r="C608">
+        <v>806409</v>
+      </c>
+      <c r="D608">
+        <v>1.8002480000000001</v>
+      </c>
+      <c r="E608">
+        <v>1.806098</v>
+      </c>
+      <c r="F608">
+        <v>1.8199449999999999</v>
+      </c>
+      <c r="G608">
+        <v>40.9</v>
+      </c>
+      <c r="H608">
+        <v>-5.1999999999999998E-3</v>
+      </c>
+      <c r="J608" t="str">
+        <f t="shared" si="9"/>
+        <v>glasses.put("S-LAH53", new GlassMap("Ohara","S-LAH53",1.806098,1.800248,1.819945)); // 40.9 806409 -0.0052</v>
+      </c>
+    </row>
+    <row r="609" spans="1:10">
+      <c r="A609" t="s">
+        <v>691</v>
+      </c>
+      <c r="B609" t="s">
+        <v>754</v>
+      </c>
+      <c r="C609">
+        <v>806409</v>
+      </c>
+      <c r="D609">
+        <v>1.8002590000000001</v>
+      </c>
+      <c r="E609">
+        <v>1.8061</v>
+      </c>
+      <c r="F609">
+        <v>1.8199540000000001</v>
+      </c>
+      <c r="G609">
+        <v>40.9</v>
+      </c>
+      <c r="H609">
+        <v>-3.8999999999999998E-3</v>
+      </c>
+      <c r="J609" t="str">
+        <f t="shared" si="9"/>
+        <v>glasses.put("S-LAH53V", new GlassMap("Ohara","S-LAH53V",1.8061,1.800259,1.819954)); // 40.9 806409 -0.0039</v>
+      </c>
+    </row>
+    <row r="610" spans="1:10">
+      <c r="A610" t="s">
+        <v>691</v>
+      </c>
+      <c r="B610" t="s">
+        <v>755</v>
+      </c>
+      <c r="C610">
+        <v>835427</v>
+      </c>
+      <c r="D610">
+        <v>1.828981</v>
+      </c>
+      <c r="E610">
+        <v>1.8348070000000001</v>
+      </c>
+      <c r="F610">
+        <v>1.8485199999999999</v>
+      </c>
+      <c r="G610">
+        <v>42.7</v>
+      </c>
+      <c r="H610">
+        <v>-7.4999999999999997E-3</v>
+      </c>
+      <c r="J610" t="str">
+        <f t="shared" si="9"/>
+        <v>glasses.put("S-LAH55V", new GlassMap("Ohara","S-LAH55V",1.834807,1.828981,1.84852)); // 42.7 835427 -0.0075</v>
+      </c>
+    </row>
+    <row r="611" spans="1:10">
+      <c r="A611" t="s">
+        <v>691</v>
+      </c>
+      <c r="B611" t="s">
+        <v>756</v>
+      </c>
+      <c r="C611">
+        <v>835427</v>
+      </c>
+      <c r="D611">
+        <v>1.8289880000000001</v>
+      </c>
+      <c r="E611">
+        <v>1.8348100000000001</v>
+      </c>
+      <c r="F611">
+        <v>1.848519</v>
+      </c>
+      <c r="G611">
+        <v>42.7</v>
+      </c>
+      <c r="H611">
+        <v>-7.4999999999999997E-3</v>
+      </c>
+      <c r="J611" t="str">
+        <f t="shared" si="9"/>
+        <v>glasses.put("S-LAH55VS", new GlassMap("Ohara","S-LAH55VS",1.83481,1.828988,1.848519)); // 42.7 835427 -0.0075</v>
+      </c>
+    </row>
+    <row r="612" spans="1:10">
+      <c r="A612" t="s">
+        <v>691</v>
+      </c>
+      <c r="B612" t="s">
+        <v>757</v>
+      </c>
+      <c r="C612">
+        <v>883408</v>
+      </c>
+      <c r="D612">
+        <v>1.87656</v>
+      </c>
+      <c r="E612">
+        <v>1.882997</v>
+      </c>
+      <c r="F612">
+        <v>1.8982209999999999</v>
+      </c>
+      <c r="G612">
+        <v>40.799999999999997</v>
+      </c>
+      <c r="H612">
+        <v>-8.8000000000000005E-3</v>
+      </c>
+      <c r="J612" t="str">
+        <f t="shared" si="9"/>
+        <v>glasses.put("S-LAH58", new GlassMap("Ohara","S-LAH58",1.882997,1.87656,1.898221)); // 40.8 883408 -0.0088</v>
+      </c>
+    </row>
+    <row r="613" spans="1:10">
+      <c r="A613" t="s">
+        <v>691</v>
+      </c>
+      <c r="B613" t="s">
+        <v>758</v>
+      </c>
+      <c r="C613">
+        <v>816466</v>
+      </c>
+      <c r="D613">
+        <v>1.8107489999999999</v>
+      </c>
+      <c r="E613">
+        <v>1.8160000000000001</v>
+      </c>
+      <c r="F613">
+        <v>1.828252</v>
+      </c>
+      <c r="G613">
+        <v>46.6</v>
+      </c>
+      <c r="H613">
+        <v>-9.1999999999999998E-3</v>
+      </c>
+      <c r="J613" t="str">
+        <f t="shared" si="9"/>
+        <v>glasses.put("S-LAH59", new GlassMap("Ohara","S-LAH59",1.816,1.810749,1.828252)); // 46.6 816466 -0.0092</v>
+      </c>
+    </row>
+    <row r="614" spans="1:10">
+      <c r="A614" t="s">
+        <v>691</v>
+      </c>
+      <c r="B614" t="s">
+        <v>759</v>
+      </c>
+      <c r="C614">
+        <v>834372</v>
+      </c>
+      <c r="D614">
+        <v>1.8273759999999999</v>
+      </c>
+      <c r="E614">
+        <v>1.8340000000000001</v>
+      </c>
+      <c r="F614">
+        <v>1.8498190000000001</v>
+      </c>
+      <c r="G614">
+        <v>37.200000000000003</v>
+      </c>
+      <c r="H614">
+        <v>-3.7000000000000002E-3</v>
+      </c>
+      <c r="J614" t="str">
+        <f t="shared" si="9"/>
+        <v>glasses.put("S-LAH60", new GlassMap("Ohara","S-LAH60",1.834,1.827376,1.849819)); // 37.2 834372 -0.0037</v>
+      </c>
+    </row>
+    <row r="615" spans="1:10">
+      <c r="A615" t="s">
+        <v>691</v>
+      </c>
+      <c r="B615" t="s">
+        <v>760</v>
+      </c>
+      <c r="C615">
+        <v>834372</v>
+      </c>
+      <c r="D615">
+        <v>1.8273919999999999</v>
+      </c>
+      <c r="E615">
+        <v>1.8340000000000001</v>
+      </c>
+      <c r="F615">
+        <v>1.8498289999999999</v>
+      </c>
+      <c r="G615">
+        <v>37.200000000000003</v>
+      </c>
+      <c r="H615">
+        <v>-2.7000000000000001E-3</v>
+      </c>
+      <c r="J615" t="str">
+        <f t="shared" si="9"/>
+        <v>glasses.put("S-LAH60MQ", new GlassMap("Ohara","S-LAH60MQ",1.834,1.827392,1.849829)); // 37.2 834372 -0.0027</v>
+      </c>
+    </row>
+    <row r="616" spans="1:10">
+      <c r="A616" t="s">
+        <v>691</v>
+      </c>
+      <c r="B616" t="s">
+        <v>761</v>
+      </c>
+      <c r="C616">
+        <v>834372</v>
+      </c>
+      <c r="D616">
+        <v>1.827399</v>
+      </c>
+      <c r="E616">
+        <v>1.8340000000000001</v>
+      </c>
+      <c r="F616">
+        <v>1.849815</v>
+      </c>
+      <c r="G616">
+        <v>37.200000000000003</v>
+      </c>
+      <c r="H616">
+        <v>-5.9999999999999995E-4</v>
+      </c>
+      <c r="J616" t="str">
+        <f t="shared" si="9"/>
+        <v>glasses.put("S-LAH60V", new GlassMap("Ohara","S-LAH60V",1.834,1.827399,1.849815)); // 37.2 834372 -0.0006</v>
+      </c>
+    </row>
+    <row r="617" spans="1:10">
+      <c r="A617" t="s">
+        <v>691</v>
+      </c>
+      <c r="B617" t="s">
+        <v>762</v>
+      </c>
+      <c r="C617">
+        <v>804396</v>
+      </c>
+      <c r="D617">
+        <v>1.798397</v>
+      </c>
+      <c r="E617">
+        <v>1.8044</v>
+      </c>
+      <c r="F617">
+        <v>1.8187199999999999</v>
+      </c>
+      <c r="G617">
+        <v>39.6</v>
+      </c>
+      <c r="H617">
+        <v>-1.1999999999999999E-3</v>
+      </c>
+      <c r="J617" t="str">
+        <f t="shared" si="9"/>
+        <v>glasses.put("S-LAH63Q", new GlassMap("Ohara","S-LAH63Q",1.8044,1.798397,1.81872)); // 39.6 804396 -0.0012</v>
+      </c>
+    </row>
+    <row r="618" spans="1:10">
+      <c r="A618" t="s">
+        <v>691</v>
+      </c>
+      <c r="B618" t="s">
+        <v>763</v>
+      </c>
+      <c r="C618">
+        <v>788474</v>
+      </c>
+      <c r="D618">
+        <v>1.7829980000000001</v>
+      </c>
+      <c r="E618">
+        <v>1.788001</v>
+      </c>
+      <c r="F618">
+        <v>1.799634</v>
+      </c>
+      <c r="G618">
+        <v>47.4</v>
+      </c>
+      <c r="H618">
+        <v>-8.8999999999999999E-3</v>
+      </c>
+      <c r="J618" t="str">
+        <f t="shared" si="9"/>
+        <v>glasses.put("S-LAH64", new GlassMap("Ohara","S-LAH64",1.788001,1.782998,1.799634)); // 47.4 788474 -0.0089</v>
+      </c>
+    </row>
+    <row r="619" spans="1:10">
+      <c r="A619" t="s">
+        <v>691</v>
+      </c>
+      <c r="B619" t="s">
+        <v>764</v>
+      </c>
+      <c r="C619">
+        <v>804466</v>
+      </c>
+      <c r="D619">
+        <v>1.7988170000000001</v>
+      </c>
+      <c r="E619">
+        <v>1.804</v>
+      </c>
+      <c r="F619">
+        <v>1.816076</v>
+      </c>
+      <c r="G619">
+        <v>46.6</v>
+      </c>
+      <c r="H619">
+        <v>-8.8000000000000005E-3</v>
+      </c>
+      <c r="J619" t="str">
+        <f t="shared" si="9"/>
+        <v>glasses.put("S-LAH65V", new GlassMap("Ohara","S-LAH65V",1.804,1.798817,1.816076)); // 46.6 804466 -0.0088</v>
+      </c>
+    </row>
+    <row r="620" spans="1:10">
+      <c r="A620" t="s">
+        <v>691</v>
+      </c>
+      <c r="B620" t="s">
+        <v>765</v>
+      </c>
+      <c r="C620">
+        <v>804465</v>
+      </c>
+      <c r="D620">
+        <v>1.798816</v>
+      </c>
+      <c r="E620">
+        <v>1.804</v>
+      </c>
+      <c r="F620">
+        <v>1.8160970000000001</v>
+      </c>
+      <c r="G620">
+        <v>46.5</v>
+      </c>
+      <c r="H620">
+        <v>-8.5000000000000006E-3</v>
+      </c>
+      <c r="J620" t="str">
+        <f t="shared" si="9"/>
+        <v>glasses.put("S-LAH65VS", new GlassMap("Ohara","S-LAH65VS",1.804,1.798816,1.816097)); // 46.5 804465 -0.0085</v>
+      </c>
+    </row>
+    <row r="621" spans="1:10">
+      <c r="A621" t="s">
+        <v>691</v>
+      </c>
+      <c r="B621" t="s">
+        <v>766</v>
+      </c>
+      <c r="C621">
+        <v>773496</v>
+      </c>
+      <c r="D621">
+        <v>1.767798</v>
+      </c>
+      <c r="E621">
+        <v>1.772499</v>
+      </c>
+      <c r="F621">
+        <v>1.783374</v>
+      </c>
+      <c r="G621">
+        <v>49.6</v>
+      </c>
+      <c r="H621">
+        <v>-9.1999999999999998E-3</v>
+      </c>
+      <c r="J621" t="str">
+        <f t="shared" si="9"/>
+        <v>glasses.put("S-LAH66", new GlassMap("Ohara","S-LAH66",1.772499,1.767798,1.783374)); // 49.6 773496 -0.0092</v>
+      </c>
+    </row>
+    <row r="622" spans="1:10">
+      <c r="A622" t="s">
+        <v>691</v>
+      </c>
+      <c r="B622" t="s">
+        <v>767</v>
+      </c>
+      <c r="C622">
+        <v>773496</v>
+      </c>
+      <c r="D622">
+        <v>1.767792</v>
+      </c>
+      <c r="E622">
+        <v>1.772499</v>
+      </c>
+      <c r="F622">
+        <v>1.7833829999999999</v>
+      </c>
+      <c r="G622">
+        <v>49.6</v>
+      </c>
+      <c r="H622">
+        <v>-9.4000000000000004E-3</v>
+      </c>
+      <c r="J622" t="str">
+        <f t="shared" si="9"/>
+        <v>glasses.put("S-LAH66N", new GlassMap("Ohara","S-LAH66N",1.772499,1.767792,1.783383)); // 49.6 773496 -0.0094</v>
+      </c>
+    </row>
+    <row r="623" spans="1:10">
+      <c r="A623" t="s">
+        <v>691</v>
+      </c>
+      <c r="B623" t="s">
+        <v>768</v>
+      </c>
+      <c r="C623">
+        <v>850323</v>
+      </c>
+      <c r="D623">
+        <v>1.8425860000000001</v>
+      </c>
+      <c r="E623">
+        <v>1.8502590000000001</v>
+      </c>
+      <c r="F623">
+        <v>1.868935</v>
+      </c>
+      <c r="G623">
+        <v>32.299999999999997</v>
+      </c>
+      <c r="H623">
+        <v>3.5999999999999999E-3</v>
+      </c>
+      <c r="J623" t="str">
+        <f t="shared" si="9"/>
+        <v>glasses.put("S-LAH71", new GlassMap("Ohara","S-LAH71",1.850259,1.842586,1.868935)); // 32.3 850323 0.0036</v>
+      </c>
+    </row>
+    <row r="624" spans="1:10">
+      <c r="A624" t="s">
+        <v>691</v>
+      </c>
+      <c r="B624" t="s">
+        <v>769</v>
+      </c>
+      <c r="C624">
+        <v>3283</v>
+      </c>
+      <c r="D624">
+        <v>1.9930110000000001</v>
+      </c>
+      <c r="E624">
+        <v>2.0032999999999999</v>
+      </c>
+      <c r="F624">
+        <v>2.0284970000000002</v>
+      </c>
+      <c r="G624">
+        <v>28.3</v>
+      </c>
+      <c r="H624">
+        <v>2.3E-3</v>
+      </c>
+      <c r="J624" t="str">
+        <f t="shared" si="9"/>
+        <v>glasses.put("S-LAH79", new GlassMap("Ohara","S-LAH79",2.0033,1.993011,2.028497)); // 28.3 3283 0.0023</v>
+      </c>
+    </row>
+    <row r="625" spans="1:10">
+      <c r="A625" t="s">
+        <v>691</v>
+      </c>
+      <c r="B625" t="s">
+        <v>770</v>
+      </c>
+      <c r="C625">
+        <v>917316</v>
+      </c>
+      <c r="D625">
+        <v>1.9080349999999999</v>
+      </c>
+      <c r="E625">
+        <v>1.9165000000000001</v>
+      </c>
+      <c r="F625">
+        <v>1.9370339999999999</v>
+      </c>
+      <c r="G625">
+        <v>31.6</v>
+      </c>
+      <c r="H625">
+        <v>8.0000000000000004E-4</v>
+      </c>
+      <c r="J625" t="str">
+        <f t="shared" si="9"/>
+        <v>glasses.put("S-LAH88", new GlassMap("Ohara","S-LAH88",1.9165,1.908035,1.937034)); // 31.6 917316 0.0008</v>
+      </c>
+    </row>
+    <row r="626" spans="1:10">
+      <c r="A626" t="s">
+        <v>691</v>
+      </c>
+      <c r="B626" t="s">
+        <v>771</v>
+      </c>
+      <c r="C626">
+        <v>852408</v>
+      </c>
+      <c r="D626">
+        <v>1.8453040000000001</v>
+      </c>
+      <c r="E626">
+        <v>1.8514999999999999</v>
+      </c>
+      <c r="F626">
+        <v>1.8661840000000001</v>
+      </c>
+      <c r="G626">
+        <v>40.799999999999997</v>
+      </c>
+      <c r="H626">
+        <v>-6.0000000000000001E-3</v>
+      </c>
+      <c r="J626" t="str">
+        <f t="shared" si="9"/>
+        <v>glasses.put("S-LAH89", new GlassMap("Ohara","S-LAH89",1.8515,1.845304,1.866184)); // 40.8 852408 -0.006</v>
+      </c>
+    </row>
+    <row r="627" spans="1:10">
+      <c r="A627" t="s">
+        <v>691</v>
+      </c>
+      <c r="B627" t="s">
+        <v>772</v>
+      </c>
+      <c r="C627">
+        <v>892371</v>
+      </c>
+      <c r="D627">
+        <v>1.8848240000000001</v>
+      </c>
+      <c r="E627">
+        <v>1.8918999999999999</v>
+      </c>
+      <c r="F627">
+        <v>1.9088430000000001</v>
+      </c>
+      <c r="G627">
+        <v>37.1</v>
+      </c>
+      <c r="H627">
+        <v>-3.3999999999999998E-3</v>
+      </c>
+      <c r="J627" t="str">
+        <f t="shared" si="9"/>
+        <v>glasses.put("S-LAH92", new GlassMap("Ohara","S-LAH92",1.8919,1.884824,1.908843)); // 37.1 892371 -0.0034</v>
+      </c>
+    </row>
+    <row r="628" spans="1:10">
+      <c r="A628" t="s">
+        <v>691</v>
+      </c>
+      <c r="B628" t="s">
+        <v>773</v>
+      </c>
+      <c r="C628">
+        <v>905350</v>
+      </c>
+      <c r="D628">
+        <v>1.8976770000000001</v>
+      </c>
+      <c r="E628">
+        <v>1.9052500000000001</v>
+      </c>
+      <c r="F628">
+        <v>1.9235150000000001</v>
+      </c>
+      <c r="G628">
+        <v>35</v>
+      </c>
+      <c r="H628">
+        <v>0</v>
+      </c>
+      <c r="J628" t="str">
+        <f t="shared" si="9"/>
+        <v>glasses.put("S-LAH93", new GlassMap("Ohara","S-LAH93",1.90525,1.897677,1.923515)); // 35 905350 0</v>
+      </c>
+    </row>
+    <row r="629" spans="1:10">
+      <c r="A629" t="s">
+        <v>691</v>
+      </c>
+      <c r="B629" t="s">
+        <v>774</v>
+      </c>
+      <c r="C629">
+        <v>904313</v>
+      </c>
+      <c r="D629">
+        <v>1.8952770000000001</v>
+      </c>
+      <c r="E629">
+        <v>1.9036599999999999</v>
+      </c>
+      <c r="F629">
+        <v>1.9241090000000001</v>
+      </c>
+      <c r="G629">
+        <v>31.3</v>
+      </c>
+      <c r="H629">
+        <v>5.4999999999999997E-3</v>
+      </c>
+      <c r="J629" t="str">
+        <f t="shared" si="9"/>
+        <v>glasses.put("S-LAH95", new GlassMap("Ohara","S-LAH95",1.90366,1.895277,1.924109)); // 31.3 904313 0.0055</v>
+      </c>
+    </row>
+    <row r="630" spans="1:10">
+      <c r="A630" t="s">
+        <v>691</v>
+      </c>
+      <c r="B630" t="s">
+        <v>775</v>
+      </c>
+      <c r="C630">
+        <v>764485</v>
+      </c>
+      <c r="D630">
+        <v>1.7591289999999999</v>
+      </c>
+      <c r="E630">
+        <v>1.7638499999999999</v>
+      </c>
+      <c r="F630">
+        <v>1.7748820000000001</v>
+      </c>
+      <c r="G630">
+        <v>48.5</v>
+      </c>
+      <c r="H630">
+        <v>-4.1000000000000003E-3</v>
+      </c>
+      <c r="J630" t="str">
+        <f t="shared" si="9"/>
+        <v>glasses.put("S-LAH96", new GlassMap("Ohara","S-LAH96",1.76385,1.759129,1.774882)); // 48.5 764485 -0.0041</v>
+      </c>
+    </row>
+    <row r="631" spans="1:10">
+      <c r="A631" t="s">
+        <v>691</v>
+      </c>
+      <c r="B631" t="s">
+        <v>776</v>
+      </c>
+      <c r="C631">
+        <v>755523</v>
+      </c>
+      <c r="D631">
+        <v>1.7506269999999999</v>
+      </c>
+      <c r="E631">
+        <v>1.7549999999999999</v>
+      </c>
+      <c r="F631">
+        <v>1.765058</v>
+      </c>
+      <c r="G631">
+        <v>52.3</v>
+      </c>
+      <c r="H631">
+        <v>-9.4000000000000004E-3</v>
+      </c>
+      <c r="J631" t="str">
+        <f t="shared" si="9"/>
+        <v>glasses.put("S-LAH97", new GlassMap("Ohara","S-LAH97",1.755,1.750627,1.765058)); // 52.3 755523 -0.0094</v>
+      </c>
+    </row>
+    <row r="632" spans="1:10">
+      <c r="A632" t="s">
+        <v>691</v>
+      </c>
+      <c r="B632" t="s">
+        <v>777</v>
+      </c>
+      <c r="C632">
+        <v>954323</v>
+      </c>
+      <c r="D632">
+        <v>1.945141</v>
+      </c>
+      <c r="E632">
+        <v>1.9537500000000001</v>
+      </c>
+      <c r="F632">
+        <v>1.974647</v>
+      </c>
+      <c r="G632">
+        <v>32.299999999999997</v>
+      </c>
+      <c r="H632">
+        <v>1.2999999999999999E-3</v>
+      </c>
+      <c r="J632" t="str">
+        <f t="shared" si="9"/>
+        <v>glasses.put("S-LAH98", new GlassMap("Ohara","S-LAH98",1.95375,1.945141,1.974647)); // 32.3 954323 0.0013</v>
+      </c>
+    </row>
+    <row r="633" spans="1:10">
+      <c r="A633" t="s">
+        <v>691</v>
+      </c>
+      <c r="B633" t="s">
+        <v>778</v>
+      </c>
+      <c r="C633">
+        <v>1291</v>
+      </c>
+      <c r="D633">
+        <v>1.9910479999999999</v>
+      </c>
+      <c r="E633">
+        <v>2.0009999999999999</v>
+      </c>
+      <c r="F633">
+        <v>2.0253999999999999</v>
+      </c>
+      <c r="G633">
+        <v>29.1</v>
+      </c>
+      <c r="H633">
+        <v>5.4000000000000003E-3</v>
+      </c>
+      <c r="J633" t="str">
+        <f t="shared" si="9"/>
+        <v>glasses.put("S-LAH99", new GlassMap("Ohara","S-LAH99",2.001,1.991048,2.0254)); // 29.1 1291 0.0054</v>
+      </c>
+    </row>
+    <row r="634" spans="1:10">
+      <c r="A634" t="s">
+        <v>691</v>
+      </c>
+      <c r="B634" t="s">
+        <v>779</v>
+      </c>
+      <c r="C634">
+        <v>1291</v>
+      </c>
+      <c r="D634">
+        <v>1.9910479999999999</v>
+      </c>
+      <c r="E634">
+        <v>2.0009999999999999</v>
+      </c>
+      <c r="F634">
+        <v>2.0253999999999999</v>
+      </c>
+      <c r="G634">
+        <v>29.1</v>
+      </c>
+      <c r="H634">
+        <v>5.4000000000000003E-3</v>
+      </c>
+      <c r="J634" t="str">
+        <f t="shared" si="9"/>
+        <v>glasses.put("S-LAH99W", new GlassMap("Ohara","S-LAH99W",2.001,1.991048,2.0254)); // 29.1 1291 0.0054</v>
+      </c>
+    </row>
+    <row r="635" spans="1:10">
+      <c r="A635" t="s">
+        <v>691</v>
+      </c>
+      <c r="B635" t="s">
+        <v>780</v>
+      </c>
+      <c r="C635">
+        <v>593353</v>
+      </c>
+      <c r="D635">
+        <v>1.5877950000000001</v>
+      </c>
+      <c r="E635">
+        <v>1.5927009999999999</v>
+      </c>
+      <c r="F635">
+        <v>1.6045799999999999</v>
+      </c>
+      <c r="G635">
+        <v>35.299999999999997</v>
+      </c>
+      <c r="H635">
+        <v>8.9999999999999993E-3</v>
+      </c>
+      <c r="J635" t="str">
+        <f t="shared" si="9"/>
+        <v>glasses.put("S-FTM16", new GlassMap("Ohara","S-FTM16",1.592701,1.587795,1.60458)); // 35.3 593353 0.009</v>
+      </c>
+    </row>
+    <row r="636" spans="1:10">
+      <c r="A636" t="s">
+        <v>691</v>
+      </c>
+      <c r="B636" t="s">
+        <v>781</v>
+      </c>
+      <c r="C636">
+        <v>613443</v>
+      </c>
+      <c r="D636">
+        <v>1.609248</v>
+      </c>
+      <c r="E636">
+        <v>1.613397</v>
+      </c>
+      <c r="F636">
+        <v>1.623105</v>
+      </c>
+      <c r="G636">
+        <v>44.3</v>
+      </c>
+      <c r="H636">
+        <v>-6.4999999999999997E-3</v>
+      </c>
+      <c r="J636" t="str">
+        <f t="shared" si="9"/>
+        <v>glasses.put("S-NBM51", new GlassMap("Ohara","S-NBM51",1.613397,1.609248,1.623105)); // 44.3 613443 -0.0065</v>
+      </c>
+    </row>
+    <row r="637" spans="1:10">
+      <c r="A637" t="s">
+        <v>691</v>
+      </c>
+      <c r="B637" t="s">
+        <v>782</v>
+      </c>
+      <c r="C637">
+        <v>622411</v>
+      </c>
+      <c r="D637">
+        <v>1.6175390000000001</v>
+      </c>
+      <c r="E637">
+        <v>1.62205</v>
+      </c>
+      <c r="F637">
+        <v>1.632682</v>
+      </c>
+      <c r="G637">
+        <v>41.1</v>
+      </c>
+      <c r="H637">
+        <v>-6.0000000000000001E-3</v>
+      </c>
+      <c r="J637" t="str">
+        <f t="shared" si="9"/>
+        <v>glasses.put("S-NBM52", new GlassMap("Ohara","S-NBM52",1.62205,1.617539,1.632682)); // 41.1 622411 -0.006</v>
+      </c>
+    </row>
+    <row r="638" spans="1:10">
+      <c r="A638" t="s">
+        <v>691</v>
+      </c>
+      <c r="B638" t="s">
+        <v>821</v>
+      </c>
+      <c r="C638">
+        <v>654397</v>
+      </c>
+      <c r="D638">
+        <v>1.6492249999999999</v>
+      </c>
+      <c r="E638">
+        <v>1.654115</v>
+      </c>
+      <c r="F638">
+        <v>1.6657090000000001</v>
+      </c>
+      <c r="G638">
+        <v>39.700000000000003</v>
+      </c>
+      <c r="H638">
+        <v>-3.5999999999999999E-3</v>
+      </c>
+      <c r="J638" t="str">
+        <f t="shared" si="9"/>
+        <v>glasses.put("S-NBH5", new GlassMap("Ohara","S-NBH5",1.654115,1.649225,1.665709)); // 39.7 654397 -0.0036</v>
+      </c>
+    </row>
+    <row r="639" spans="1:10">
+      <c r="A639" t="s">
+        <v>691</v>
+      </c>
+      <c r="B639" t="s">
+        <v>820</v>
+      </c>
+      <c r="C639">
+        <v>720347</v>
+      </c>
+      <c r="D639">
+        <v>1.7143649999999999</v>
+      </c>
+      <c r="E639">
+        <v>1.720467</v>
+      </c>
+      <c r="F639">
+        <v>1.735123</v>
+      </c>
+      <c r="G639">
+        <v>34.700000000000003</v>
+      </c>
+      <c r="H639">
+        <v>-1.9E-3</v>
+      </c>
+      <c r="J639" t="str">
+        <f t="shared" si="9"/>
+        <v>glasses.put("S-NBH8", new GlassMap("Ohara","S-NBH8",1.720467,1.714365,1.735123)); // 34.7 720347 -0.0019</v>
+      </c>
+    </row>
+    <row r="640" spans="1:10">
+      <c r="A640" t="s">
+        <v>691</v>
+      </c>
+      <c r="B640" t="s">
+        <v>783</v>
+      </c>
+      <c r="C640">
+        <v>750353</v>
+      </c>
+      <c r="D640">
+        <v>1.7432589999999999</v>
+      </c>
+      <c r="E640">
+        <v>1.7495050000000001</v>
+      </c>
+      <c r="F640">
+        <v>1.764473</v>
+      </c>
+      <c r="G640">
+        <v>35.299999999999997</v>
+      </c>
+      <c r="H640">
+        <v>-2.5000000000000001E-3</v>
+      </c>
+      <c r="J640" t="str">
+        <f t="shared" si="9"/>
+        <v>glasses.put("S-NBH51", new GlassMap("Ohara","S-NBH51",1.749505,1.743259,1.764473)); // 35.3 750353 -0.0025</v>
+      </c>
+    </row>
+    <row r="641" spans="1:10">
+      <c r="A641" t="s">
+        <v>691</v>
+      </c>
+      <c r="B641" t="s">
+        <v>784</v>
+      </c>
+      <c r="C641">
+        <v>673383</v>
+      </c>
+      <c r="D641">
+        <v>1.6677919999999999</v>
+      </c>
+      <c r="E641">
+        <v>1.673</v>
+      </c>
+      <c r="F641">
+        <v>1.685384</v>
+      </c>
+      <c r="G641">
+        <v>38.299999999999997</v>
+      </c>
+      <c r="H641">
+        <v>-3.8999999999999998E-3</v>
+      </c>
+      <c r="J641" t="str">
+        <f t="shared" si="9"/>
+        <v>glasses.put("S-NBH52V", new GlassMap("Ohara","S-NBH52V",1.673,1.667792,1.685384)); // 38.3 673383 -0.0039</v>
+      </c>
+    </row>
+    <row r="642" spans="1:10">
+      <c r="A642" t="s">
+        <v>691</v>
+      </c>
+      <c r="B642" t="s">
+        <v>785</v>
+      </c>
+      <c r="C642">
+        <v>738323</v>
+      </c>
+      <c r="D642">
+        <v>1.731322</v>
+      </c>
+      <c r="E642">
+        <v>1.738</v>
+      </c>
+      <c r="F642">
+        <v>1.7541519999999999</v>
+      </c>
+      <c r="G642">
+        <v>32.299999999999997</v>
+      </c>
+      <c r="H642">
+        <v>8.0000000000000004E-4</v>
+      </c>
+      <c r="J642" t="str">
+        <f t="shared" si="9"/>
+        <v>glasses.put("S-NBH53V", new GlassMap("Ohara","S-NBH53V",1.738,1.731322,1.754152)); // 32.3 738323 0.0008</v>
+      </c>
+    </row>
+    <row r="643" spans="1:10">
+      <c r="A643" t="s">
+        <v>691</v>
+      </c>
+      <c r="B643" t="s">
+        <v>786</v>
+      </c>
+      <c r="C643">
+        <v>800299</v>
+      </c>
+      <c r="D643">
+        <v>1.7922370000000001</v>
+      </c>
+      <c r="E643">
+        <v>1.8</v>
+      </c>
+      <c r="F643">
+        <v>1.819043</v>
+      </c>
+      <c r="G643">
+        <v>29.9</v>
+      </c>
+      <c r="H643">
+        <v>8.5000000000000006E-3</v>
+      </c>
+      <c r="J643" t="str">
+        <f t="shared" ref="J643:J654" si="10">CONCATENATE("glasses.put(""",B643,""", new GlassMap(""",A643,""",""",B643,""",",E643,",",D643,",",F643,")); // ",G643, " ",C643," ",H643)</f>
+        <v>glasses.put("S-NBH55", new GlassMap("Ohara","S-NBH55",1.8,1.792237,1.819043)); // 29.9 800299 0.0085</v>
+      </c>
+    </row>
+    <row r="644" spans="1:10">
+      <c r="A644" t="s">
+        <v>691</v>
+      </c>
+      <c r="B644" t="s">
+        <v>787</v>
+      </c>
+      <c r="C644">
+        <v>855248</v>
+      </c>
+      <c r="D644">
+        <v>1.844876</v>
+      </c>
+      <c r="E644">
+        <v>1.8547800000000001</v>
+      </c>
+      <c r="F644">
+        <v>1.879345</v>
+      </c>
+      <c r="G644">
+        <v>24.8</v>
+      </c>
+      <c r="H644">
+        <v>1.09E-2</v>
+      </c>
+      <c r="J644" t="str">
+        <f t="shared" si="10"/>
+        <v>glasses.put("S-NBH56", new GlassMap("Ohara","S-NBH56",1.85478,1.844876,1.879345)); // 24.8 855248 0.0109</v>
+      </c>
+    </row>
+    <row r="645" spans="1:10">
+      <c r="A645" t="s">
+        <v>691</v>
+      </c>
+      <c r="B645" t="s">
+        <v>788</v>
+      </c>
+      <c r="C645">
+        <v>850300</v>
+      </c>
+      <c r="D645">
+        <v>1.8420369999999999</v>
+      </c>
+      <c r="E645">
+        <v>1.85025</v>
+      </c>
+      <c r="F645">
+        <v>1.870336</v>
+      </c>
+      <c r="G645">
+        <v>30</v>
+      </c>
+      <c r="H645">
+        <v>5.1000000000000004E-3</v>
+      </c>
+      <c r="J645" t="str">
+        <f t="shared" si="10"/>
+        <v>glasses.put("S-NBH57", new GlassMap("Ohara","S-NBH57",1.85025,1.842037,1.870336)); // 30 850300 0.0051</v>
+      </c>
+    </row>
+    <row r="646" spans="1:10">
+      <c r="A646" t="s">
+        <v>691</v>
+      </c>
+      <c r="B646" t="s">
+        <v>789</v>
+      </c>
+      <c r="C646">
+        <v>789284</v>
+      </c>
+      <c r="D646">
+        <v>1.7807569999999999</v>
+      </c>
+      <c r="E646">
+        <v>1.7887999999999999</v>
+      </c>
+      <c r="F646">
+        <v>1.8085039999999999</v>
+      </c>
+      <c r="G646">
+        <v>28.4</v>
+      </c>
+      <c r="H646">
+        <v>5.4000000000000003E-3</v>
+      </c>
+      <c r="J646" t="str">
+        <f t="shared" si="10"/>
+        <v>glasses.put("S-NBH58", new GlassMap("Ohara","S-NBH58",1.7888,1.780757,1.808504)); // 28.4 789284 0.0054</v>
+      </c>
+    </row>
+    <row r="647" spans="1:10">
+      <c r="A647" t="s">
+        <v>691</v>
+      </c>
+      <c r="B647" t="s">
+        <v>790</v>
+      </c>
+      <c r="C647">
+        <v>766358</v>
+      </c>
+      <c r="D647">
+        <v>1.7600389999999999</v>
+      </c>
+      <c r="E647">
+        <v>1.7663420000000001</v>
+      </c>
+      <c r="F647">
+        <v>1.7814319999999999</v>
+      </c>
+      <c r="G647">
+        <v>35.799999999999997</v>
+      </c>
+      <c r="H647">
+        <v>-4.3E-3</v>
+      </c>
+      <c r="J647" t="str">
+        <f t="shared" si="10"/>
+        <v>glasses.put("S-NBH59", new GlassMap("Ohara","S-NBH59",1.766342,1.760039,1.781432)); // 35.8 766358 -0.0043</v>
+      </c>
+    </row>
+    <row r="648" spans="1:10">
+      <c r="A648" t="s">
+        <v>691</v>
+      </c>
+      <c r="B648" t="s">
+        <v>813</v>
+      </c>
+      <c r="C648">
+        <v>808228</v>
+      </c>
+      <c r="D648">
+        <v>1.798009</v>
+      </c>
+      <c r="E648">
+        <v>1.808095</v>
+      </c>
+      <c r="F648">
+        <v>1.8335129999999999</v>
+      </c>
+      <c r="G648">
+        <v>22.8</v>
+      </c>
+      <c r="H648">
+        <v>2.6100000000000002E-2</v>
+      </c>
+      <c r="J648" t="str">
+        <f t="shared" si="10"/>
+        <v>glasses.put("S-NPH1", new GlassMap("Ohara","S-NPH1",1.808095,1.798009,1.833513)); // 22.8 808228 0.0261</v>
+      </c>
+    </row>
+    <row r="649" spans="1:10">
+      <c r="A649" t="s">
+        <v>691</v>
+      </c>
+      <c r="B649" t="s">
+        <v>814</v>
+      </c>
+      <c r="C649">
+        <v>808228</v>
+      </c>
+      <c r="D649">
+        <v>1.798009</v>
+      </c>
+      <c r="E649">
+        <v>1.808095</v>
+      </c>
+      <c r="F649">
+        <v>1.8335129999999999</v>
+      </c>
+      <c r="G649">
+        <v>22.8</v>
+      </c>
+      <c r="H649">
+        <v>2.6100000000000002E-2</v>
+      </c>
+      <c r="J649" t="str">
+        <f t="shared" si="10"/>
+        <v>glasses.put("S-NPH1W", new GlassMap("Ohara","S-NPH1W",1.808095,1.798009,1.833513)); // 22.8 808228 0.0261</v>
+      </c>
+    </row>
+    <row r="650" spans="1:10">
+      <c r="A650" t="s">
+        <v>691</v>
+      </c>
+      <c r="B650" t="s">
+        <v>815</v>
+      </c>
+      <c r="C650">
+        <v>923189</v>
+      </c>
+      <c r="D650">
+        <v>1.9091579999999999</v>
+      </c>
+      <c r="E650">
+        <v>1.92286</v>
+      </c>
+      <c r="F650">
+        <v>1.9579960000000001</v>
+      </c>
+      <c r="G650">
+        <v>18.899999999999999</v>
+      </c>
+      <c r="H650">
+        <v>3.8600000000000002E-2</v>
+      </c>
+      <c r="J650" t="str">
+        <f t="shared" si="10"/>
+        <v>glasses.put("S-NPH2", new GlassMap("Ohara","S-NPH2",1.92286,1.909158,1.957996)); // 18.9 923189 0.0386</v>
+      </c>
+    </row>
+    <row r="651" spans="1:10">
+      <c r="A651" t="s">
+        <v>691</v>
+      </c>
+      <c r="B651" t="s">
+        <v>816</v>
+      </c>
+      <c r="C651">
+        <v>959175</v>
+      </c>
+      <c r="D651">
+        <v>1.9437599999999999</v>
+      </c>
+      <c r="E651">
+        <v>1.95906</v>
+      </c>
+      <c r="F651">
+        <v>1.9986550000000001</v>
+      </c>
+      <c r="G651">
+        <v>17.5</v>
+      </c>
+      <c r="H651">
+        <v>4.6600000000000003E-2</v>
+      </c>
+      <c r="J651" t="str">
+        <f t="shared" si="10"/>
+        <v>glasses.put("S-NPH3", new GlassMap("Ohara","S-NPH3",1.95906,1.94376,1.998655)); // 17.5 959175 0.0466</v>
+      </c>
+    </row>
+    <row r="652" spans="1:10">
+      <c r="A652" t="s">
+        <v>691</v>
+      </c>
+      <c r="B652" t="s">
+        <v>817</v>
+      </c>
+      <c r="C652">
+        <v>893204</v>
+      </c>
+      <c r="D652">
+        <v>1.880484</v>
+      </c>
+      <c r="E652">
+        <v>1.89286</v>
+      </c>
+      <c r="F652">
+        <v>1.9243349999999999</v>
+      </c>
+      <c r="G652">
+        <v>20.399999999999999</v>
+      </c>
+      <c r="H652">
+        <v>3.0800000000000001E-2</v>
+      </c>
+      <c r="J652" t="str">
+        <f t="shared" si="10"/>
+        <v>glasses.put("S-NPH4", new GlassMap("Ohara","S-NPH4",1.89286,1.880484,1.924335)); // 20.4 893204 0.0308</v>
+      </c>
+    </row>
+    <row r="653" spans="1:10">
+      <c r="A653" t="s">
+        <v>691</v>
+      </c>
+      <c r="B653" t="s">
+        <v>818</v>
+      </c>
+      <c r="C653">
+        <v>859227</v>
+      </c>
+      <c r="D653">
+        <v>1.848209</v>
+      </c>
+      <c r="E653">
+        <v>1.8589560000000001</v>
+      </c>
+      <c r="F653">
+        <v>1.886001</v>
+      </c>
+      <c r="G653">
+        <v>22.7</v>
+      </c>
+      <c r="H653">
+        <v>2.3699999999999999E-2</v>
+      </c>
+      <c r="J653" t="str">
+        <f t="shared" si="10"/>
+        <v>glasses.put("S-NPH5", new GlassMap("Ohara","S-NPH5",1.858956,1.848209,1.886001)); // 22.7 859227 0.0237</v>
+      </c>
+    </row>
+    <row r="654" spans="1:10">
+      <c r="A654" t="s">
+        <v>691</v>
+      </c>
+      <c r="B654" t="s">
+        <v>819</v>
+      </c>
+      <c r="C654">
+        <v>778239</v>
+      </c>
+      <c r="D654">
+        <v>1.7690239999999999</v>
+      </c>
+      <c r="E654">
+        <v>1.7783</v>
+      </c>
+      <c r="F654">
+        <v>1.8015730000000001</v>
+      </c>
+      <c r="G654">
+        <v>23.9</v>
+      </c>
+      <c r="H654">
+        <v>2.1999999999999999E-2</v>
+      </c>
+      <c r="J654" t="str">
+        <f t="shared" si="10"/>
+        <v>glasses.put("S-NPH7", new GlassMap("Ohara","S-NPH7",1.7783,1.769024,1.801573)); // 23.9 778239 0.022</v>
       </c>
     </row>
   </sheetData>

</xml_diff>